<commit_message>
vessels export template beta implemented
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement_Vessels.xlsx
+++ b/templates/Export_Agreement_Vessels.xlsx
@@ -8,133 +8,133 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3226BE2-4141-4CA3-83EC-CE7C0D54855D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD720957-086E-488C-BB32-256144E6A3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26978" yWindow="-98" windowWidth="27076" windowHeight="16395" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="-55778" yWindow="-907" windowWidth="28995" windowHeight="15795" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
     <sheet name="Com_Invoice" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Export_Contract!$A$1:$B$55</definedName>
-    <definedName name="Адреса_банк_получателя">Export_Contract!$A$41</definedName>
-    <definedName name="Адреса_банк_получателя_адрес">Export_Contract!$A$42</definedName>
-    <definedName name="Адреса_банк_получателя_свифт">Export_Contract!$A$43</definedName>
-    <definedName name="Адреса_подпись">Export_Contract!$A$55</definedName>
-    <definedName name="Адреса_покупатель">Export_Contract!$A$47</definedName>
-    <definedName name="Адреса_покупатель_адрес">Export_Contract!$A$48</definedName>
-    <definedName name="Адреса_покупатель_банк">Export_Contract!$A$49</definedName>
-    <definedName name="Адреса_покупатель_банк_адрес">Export_Contract!$A$51</definedName>
-    <definedName name="Адреса_покупатель_банк_ветвь">Export_Contract!$A$50</definedName>
-    <definedName name="Адреса_покупатель_банк_свифт">Export_Contract!$A$52</definedName>
-    <definedName name="Адреса_покупатель_бенефициар">Export_Contract!$A$53</definedName>
-    <definedName name="Адреса_покупатель_заголовок">Export_Contract!$A$46</definedName>
-    <definedName name="Адреса_покупатель_счет">Export_Contract!$A$54</definedName>
-    <definedName name="Адреса_получатель_в_пользу">Export_Contract!$A$44</definedName>
-    <definedName name="Адреса_получатель_счет">Export_Contract!$A$45</definedName>
-    <definedName name="Адреса_продавец">Export_Contract!$A$39</definedName>
-    <definedName name="Адреса_продавец_адрес">Export_Contract!$A$40</definedName>
-    <definedName name="Адреса_продавец_заголовок">Export_Contract!$A$38</definedName>
-    <definedName name="Адреса_сторон_заголовок">Export_Contract!$A$37</definedName>
-    <definedName name="Доставка_заголовок">Export_Contract!$A$29</definedName>
-    <definedName name="Доставка_порт">Export_Contract!$A$31</definedName>
-    <definedName name="Доставка_условия">Export_Contract!$A$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Export_Contract!$A$1:$B$70</definedName>
+    <definedName name="Адреса_банк_получателя">Export_Contract!$A$34</definedName>
+    <definedName name="Адреса_банк_получателя_адрес">Export_Contract!$A$35</definedName>
+    <definedName name="Адреса_банк_получателя_свифт">Export_Contract!$A$36</definedName>
+    <definedName name="Адреса_подпись">Export_Contract!$A$48</definedName>
+    <definedName name="Адреса_покупатель">Export_Contract!$A$40</definedName>
+    <definedName name="Адреса_покупатель_адрес">Export_Contract!$A$41</definedName>
+    <definedName name="Адреса_покупатель_банк">Export_Contract!$A$42</definedName>
+    <definedName name="Адреса_покупатель_банк_адрес">Export_Contract!$A$44</definedName>
+    <definedName name="Адреса_покупатель_банк_ветвь">Export_Contract!$A$43</definedName>
+    <definedName name="Адреса_покупатель_банк_свифт">Export_Contract!$A$45</definedName>
+    <definedName name="Адреса_покупатель_бенефициар">Export_Contract!$A$46</definedName>
+    <definedName name="Адреса_покупатель_заголовок">Export_Contract!$A$39</definedName>
+    <definedName name="Адреса_покупатель_счет">Export_Contract!$A$47</definedName>
+    <definedName name="Адреса_получатель_в_пользу">Export_Contract!$A$37</definedName>
+    <definedName name="Адреса_получатель_счет">Export_Contract!$A$38</definedName>
+    <definedName name="Адреса_продавец">Export_Contract!$A$32</definedName>
+    <definedName name="Адреса_продавец_адрес">Export_Contract!$A$33</definedName>
+    <definedName name="Адреса_продавец_заголовок">Export_Contract!$A$31</definedName>
+    <definedName name="Адреса_сторон_заголовок">Export_Contract!$A$30</definedName>
+    <definedName name="Доставка_заголовок">Export_Contract!$A$23</definedName>
+    <definedName name="Доставка_порт">Export_Contract!$A$25</definedName>
+    <definedName name="Доставка_условия">Export_Contract!$A$24</definedName>
     <definedName name="Инвойс">Com_Invoice!$E$4</definedName>
     <definedName name="Инвойс_Bl_массив">Com_Invoice!$A$16</definedName>
-    <definedName name="Инвойс_Bl_массив_п">Com_Invoice!$A$82</definedName>
-    <definedName name="Инвойс_банк_получателя">Com_Invoice!$A$45</definedName>
-    <definedName name="Инвойс_банк_получателя_адрес">Com_Invoice!$A$46</definedName>
-    <definedName name="Инвойс_банк_получателя_адрес_п">Com_Invoice!$A$111</definedName>
-    <definedName name="Инвойс_банк_получателя_п">Com_Invoice!$A$110</definedName>
-    <definedName name="Инвойс_банк_получателя_свифт">Com_Invoice!$A$47</definedName>
-    <definedName name="Инвойс_банк_получателя_свифт_п">Com_Invoice!$A$112</definedName>
+    <definedName name="Инвойс_Bl_массив_п">Com_Invoice!$A$81</definedName>
+    <definedName name="Инвойс_банк_получателя">Com_Invoice!$A$44</definedName>
+    <definedName name="Инвойс_банк_получателя_адрес">Com_Invoice!$A$45</definedName>
+    <definedName name="Инвойс_банк_получателя_адрес_п">Com_Invoice!$A$109</definedName>
+    <definedName name="Инвойс_банк_получателя_п">Com_Invoice!$A$108</definedName>
+    <definedName name="Инвойс_банк_получателя_свифт">Com_Invoice!$A$46</definedName>
+    <definedName name="Инвойс_банк_получателя_свифт_п">Com_Invoice!$A$110</definedName>
     <definedName name="Инвойс_всего">Com_Invoice!$F$16</definedName>
-    <definedName name="Инвойс_всего_п">Com_Invoice!$F$82</definedName>
+    <definedName name="Инвойс_всего_п">Com_Invoice!$F$81</definedName>
     <definedName name="Инвойс_дата">Com_Invoice!$A$10</definedName>
-    <definedName name="Инвойс_дата_п">Com_Invoice!$A$76</definedName>
+    <definedName name="Инвойс_дата_п">Com_Invoice!$A$75</definedName>
     <definedName name="Инвойс_декларация">Com_Invoice!$A$13</definedName>
-    <definedName name="Инвойс_декларация_п">Com_Invoice!$A$79</definedName>
+    <definedName name="Инвойс_декларация_п">Com_Invoice!$A$78</definedName>
     <definedName name="Инвойс_контракт">Com_Invoice!$E$11</definedName>
     <definedName name="Инвойс_контракт_дата">Com_Invoice!$E$12</definedName>
-    <definedName name="Инвойс_контракт_дата_п">Com_Invoice!$E$78</definedName>
-    <definedName name="Инвойс_контракт_п">Com_Invoice!$E$77</definedName>
+    <definedName name="Инвойс_контракт_дата_п">Com_Invoice!$E$77</definedName>
+    <definedName name="Инвойс_контракт_п">Com_Invoice!$E$76</definedName>
     <definedName name="Инвойс_куда">Com_Invoice!$A$12</definedName>
-    <definedName name="Инвойс_куда_п">Com_Invoice!$A$78</definedName>
+    <definedName name="Инвойс_куда_п">Com_Invoice!$A$77</definedName>
     <definedName name="Инвойс_места">Com_Invoice!$E$16</definedName>
-    <definedName name="Инвойс_места_п">Com_Invoice!$E$82</definedName>
+    <definedName name="Инвойс_места_п">Com_Invoice!$E$81</definedName>
     <definedName name="Инвойс_откуда">Com_Invoice!$B$12</definedName>
-    <definedName name="Инвойс_откуда_п">Com_Invoice!$B$78</definedName>
-    <definedName name="Инвойс_п">Com_Invoice!$E$70</definedName>
-    <definedName name="Инвойс_подвал_всего">Com_Invoice!$E$43</definedName>
-    <definedName name="Инвойс_подвал_всего_п">Com_Invoice!$E$108</definedName>
-    <definedName name="Инвойс_подвал_места">Com_Invoice!$D$43</definedName>
-    <definedName name="Инвойс_подвал_места_п">Com_Invoice!$D$108</definedName>
-    <definedName name="Инвойс_подвал_сумма">Com_Invoice!$H$43</definedName>
-    <definedName name="Инвойс_подвал_сумма_п">Com_Invoice!$H$108</definedName>
-    <definedName name="Инвойс_подписант">Com_Invoice!$E$45</definedName>
-    <definedName name="Инвойс_подписант_п">Com_Invoice!$E$110</definedName>
+    <definedName name="Инвойс_откуда_п">Com_Invoice!$B$77</definedName>
+    <definedName name="Инвойс_п">Com_Invoice!$E$69</definedName>
+    <definedName name="Инвойс_подвал_всего">Com_Invoice!$E$42</definedName>
+    <definedName name="Инвойс_подвал_всего_п">Com_Invoice!$E$106</definedName>
+    <definedName name="Инвойс_подвал_места">Com_Invoice!$D$42</definedName>
+    <definedName name="Инвойс_подвал_места_п">Com_Invoice!$D$106</definedName>
+    <definedName name="Инвойс_подвал_сумма">Com_Invoice!$H$42</definedName>
+    <definedName name="Инвойс_подвал_сумма_п">Com_Invoice!$H$106</definedName>
+    <definedName name="Инвойс_подписант">Com_Invoice!$E$44</definedName>
+    <definedName name="Инвойс_подписант_п">Com_Invoice!$E$108</definedName>
     <definedName name="Инвойс_покупатель">Com_Invoice!$E$7</definedName>
     <definedName name="Инвойс_покупатель_адрес">Com_Invoice!$E$8</definedName>
-    <definedName name="Инвойс_покупатель_адрес_п">Com_Invoice!$E$74</definedName>
-    <definedName name="Инвойс_покупатель_п">Com_Invoice!$E$73</definedName>
+    <definedName name="Инвойс_покупатель_адрес_п">Com_Invoice!$E$73</definedName>
+    <definedName name="Инвойс_покупатель_п">Com_Invoice!$E$72</definedName>
     <definedName name="Инвойс_получатель">Com_Invoice!$A$7</definedName>
     <definedName name="Инвойс_получатель_адрес">Com_Invoice!$A$8</definedName>
-    <definedName name="Инвойс_получатель_адрес_п">Com_Invoice!$A$74</definedName>
-    <definedName name="Инвойс_получатель_в_пользу">Com_Invoice!$A$48</definedName>
-    <definedName name="Инвойс_получатель_в_пользу_п">Com_Invoice!$A$113</definedName>
-    <definedName name="Инвойс_получатель_п">Com_Invoice!$A$73</definedName>
-    <definedName name="Инвойс_получатель_счет">Com_Invoice!$A$49</definedName>
-    <definedName name="Инвойс_получатель_счет_п">Com_Invoice!$A$114</definedName>
+    <definedName name="Инвойс_получатель_адрес_п">Com_Invoice!$A$73</definedName>
+    <definedName name="Инвойс_получатель_в_пользу">Com_Invoice!$A$47</definedName>
+    <definedName name="Инвойс_получатель_в_пользу_п">Com_Invoice!$A$111</definedName>
+    <definedName name="Инвойс_получатель_п">Com_Invoice!$A$72</definedName>
+    <definedName name="Инвойс_получатель_счет">Com_Invoice!$A$48</definedName>
+    <definedName name="Инвойс_получатель_счет_п">Com_Invoice!$A$112</definedName>
     <definedName name="Инвойс_продавец">Com_Invoice!$A$4</definedName>
     <definedName name="Инвойс_продавец_адрес">Com_Invoice!$A$5</definedName>
-    <definedName name="Инвойс_продавец_адрес_п">Com_Invoice!$A$71</definedName>
-    <definedName name="Инвойс_продавец_п">Com_Invoice!$A$70</definedName>
+    <definedName name="Инвойс_продавец_адрес_п">Com_Invoice!$A$70</definedName>
+    <definedName name="Инвойс_продавец_п">Com_Invoice!$A$69</definedName>
     <definedName name="Инвойс_продукт">Com_Invoice!$C$16</definedName>
-    <definedName name="Инвойс_продукт_п">Com_Invoice!$C$82</definedName>
+    <definedName name="Инвойс_продукт_п">Com_Invoice!$C$81</definedName>
     <definedName name="Инвойс_соглашение">Com_Invoice!$E$10</definedName>
-    <definedName name="Инвойс_соглашение_п">Com_Invoice!$E$76</definedName>
-    <definedName name="Инвойс_судно">Com_Invoice!$A$40</definedName>
-    <definedName name="Инвойс_судно_п">Com_Invoice!$A$105</definedName>
+    <definedName name="Инвойс_соглашение_п">Com_Invoice!$E$75</definedName>
+    <definedName name="Инвойс_судно">Com_Invoice!$A$39</definedName>
+    <definedName name="Инвойс_судно_п">Com_Invoice!$A$103</definedName>
     <definedName name="Инвойс_сумма">Com_Invoice!$H$16</definedName>
-    <definedName name="Инвойс_сумма_п">Com_Invoice!$H$82</definedName>
+    <definedName name="Инвойс_сумма_п">Com_Invoice!$H$81</definedName>
     <definedName name="Инвойс_транспорт">Com_Invoice!$B$10</definedName>
-    <definedName name="Инвойс_транспорт_п">Com_Invoice!$B$76</definedName>
+    <definedName name="Инвойс_транспорт_п">Com_Invoice!$B$75</definedName>
     <definedName name="Инвойс_упаковка">Com_Invoice!$D$16</definedName>
-    <definedName name="Инвойс_упаковка_п">Com_Invoice!$D$82</definedName>
+    <definedName name="Инвойс_упаковка_п">Com_Invoice!$D$81</definedName>
     <definedName name="Инвойс_условия">Com_Invoice!$E$14</definedName>
-    <definedName name="Инвойс_условия_п">Com_Invoice!$E$80</definedName>
+    <definedName name="Инвойс_условия_п">Com_Invoice!$E$79</definedName>
     <definedName name="Инвойс_цена">Com_Invoice!$G$16</definedName>
-    <definedName name="Инвойс_цена_п">Com_Invoice!$G$82</definedName>
+    <definedName name="Инвойс_цена_п">Com_Invoice!$G$81</definedName>
     <definedName name="Контракт">Export_Contract!$A$2</definedName>
     <definedName name="Контракт_дата">Export_Contract!$A$3</definedName>
     <definedName name="МСЦ">Com_Invoice!$G$4</definedName>
-    <definedName name="МСЦ_п">Com_Invoice!$G$70</definedName>
+    <definedName name="МСЦ_п">Com_Invoice!$G$69</definedName>
     <definedName name="МСЦ_сертификат">Com_Invoice!$H$4</definedName>
-    <definedName name="МСЦ_сертификат_п">Com_Invoice!$H$70</definedName>
+    <definedName name="МСЦ_сертификат_п">Com_Invoice!$H$69</definedName>
     <definedName name="Покупатель">Export_Contract!$A$11</definedName>
     <definedName name="Покупатель_адрес">Export_Contract!$A$12</definedName>
     <definedName name="Покупатель_заголовок">Export_Contract!$A$10</definedName>
     <definedName name="Покупатель_представитель">Export_Contract!$A$13</definedName>
     <definedName name="Покупатель_представитель_подробно">Export_Contract!$A$14</definedName>
     <definedName name="Предмет_заголовок">Export_Contract!$A$15</definedName>
-    <definedName name="Предмет_массив">Export_Contract!$A$20</definedName>
+    <definedName name="Предмет_массив">Export_Contract!$A$17</definedName>
     <definedName name="Предмет_описание">Export_Contract!$A$16</definedName>
     <definedName name="Продавец">Export_Contract!$A$6</definedName>
     <definedName name="Продавец_адрес">Export_Contract!$A$7</definedName>
     <definedName name="Продавец_заголовок">Export_Contract!$A$5</definedName>
     <definedName name="Продавец_подписант">Export_Contract!$A$9</definedName>
     <definedName name="Продавец_представитель">Export_Contract!$A$8</definedName>
-    <definedName name="Прочие_условия_заголовок">Export_Contract!$A$35</definedName>
-    <definedName name="Прочие_условия_описание">Export_Contract!$A$36</definedName>
-    <definedName name="Сертификаты_массив">Export_Contract!$A$34</definedName>
-    <definedName name="Сертификаты_описание">Export_Contract!$A$32</definedName>
+    <definedName name="Прочие_условия_заголовок">Export_Contract!$A$28</definedName>
+    <definedName name="Прочие_условия_описание">Export_Contract!$A$29</definedName>
+    <definedName name="Сертификаты_массив">Export_Contract!$A$27</definedName>
+    <definedName name="Сертификаты_описание">Export_Contract!$A$26</definedName>
     <definedName name="Соглашение">Export_Contract!$A$1</definedName>
     <definedName name="Стороны_заголовок">Export_Contract!$A$4</definedName>
-    <definedName name="Цена_всего">Export_Contract!$A$28</definedName>
-    <definedName name="Цена_заголовок">Export_Contract!$A$22</definedName>
-    <definedName name="Цена_массив">Export_Contract!$A$27</definedName>
-    <definedName name="Цена_описание">Export_Contract!$A$23</definedName>
+    <definedName name="Цена_всего">Export_Contract!$A$22</definedName>
+    <definedName name="Цена_заголовок">Export_Contract!$A$19</definedName>
+    <definedName name="Цена_массив">Export_Contract!$A$21</definedName>
+    <definedName name="Цена_описание">Export_Contract!$A$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="172">
   <si>
     <t>COMMERCIAL INVOICE</t>
   </si>
@@ -620,25 +620,6 @@
     <t>Portovaya, 1, Magadan, Russia, 685000</t>
   </si>
   <si>
-    <t>*  f/v "Morskoy Volk"
-    MSC Frozen Alaska Pollock Milts - 9,585 tn (net weight)</t>
-  </si>
-  <si>
-    <t>*  МФТ "Морской Волк"
-    MSC Молоки минтая мороженые
-    - 3 500,00 долл. за одну тонну (нетто)</t>
-  </si>
-  <si>
-    <t>*  f/v "Morskoy Volk" 
-    MSC Frozen Alaska Pollock Milts 
-    - USD 3 500,00 for one tn net weight</t>
-  </si>
-  <si>
-    <t>*  f/v "Morskoy Volk"
-    MSC Frozen Alaska Pollock Milts
-    - USD 3 500,00 for one tn net weight</t>
-  </si>
-  <si>
     <t>Декларация (Если EXW)</t>
   </si>
   <si>
@@ -654,54 +635,46 @@
     <t>Изготовитель</t>
   </si>
   <si>
-    <t>СРТМ "Си Хантер"</t>
-  </si>
-  <si>
-    <t>f/v "Sea Hunter"</t>
-  </si>
-  <si>
     <t>Страна происхождения РОССИЯ</t>
-  </si>
-  <si>
-    <t>*  МФТ "Морской Волк"
-    MSC Молоки минтая мороженные - 9,585 тн (нетто)</t>
-  </si>
-  <si>
-    <t>*  f/v "Sea Hunter"
-    MSC Frozen Alaska Pollock Roe- 0,150 tn (net weight)</t>
-  </si>
-  <si>
-    <t>*  СРТМ "Си Хантер"
-    MSC Икра минтая - 0,150 тн (нетто)</t>
-  </si>
-  <si>
-    <t>*  f/v "Morskoy Volk"
-    MSC Frozen Alaska Pollock Milts- 29,585 tn (net weight)</t>
-  </si>
-  <si>
-    <t>*  МФТ "Морской Волк"
-    MSC Молоки минтая мороженые - 29,585 тн (нетто)</t>
-  </si>
-  <si>
-    <t>*  f/v "Sea Hunter"
-    MSC Frozen Alaska Pollock Roe - 222,021 tn (net weight)</t>
   </si>
   <si>
     <t>*  МФТ "Морской Волк"
     MSC Икра минтая - 222,021 тн (нетто)</t>
   </si>
   <si>
-    <t>*  МФТ "Морской Волк"
-    MSC Молоки минтая мороженные
-    - 3 500,00 долл. за одну тонну (нетто)</t>
-  </si>
-  <si>
-    <t>1) MARINE RENAISSANCE CO. LTD 
-ROOM 1105, NOBLIAN2, 80, JUNGANG-DAERO, JUNG-GU, BUSAN, KOREA
-*  f/v "Morskoy Volk"
-    MSC Frozen Alaska Pollock Milts - 9,585 tn (net weight)
-*  f/v "Sea Hunter"
-    MSC Frozen Alaska Pollock Roe - 0,150 tn (net weight)</t>
+    <t>*  f/v "Sea Hunter"
+    MSC Frozen Alaska Pollock Roe
+    - USD 4 500,00 for one tn net weight</t>
+  </si>
+  <si>
+    <t>*  СРТМ "Си Хантер"
+    MSC Икра минтая 
+    - 4 500,00 долл. за одну тонну (нетто)</t>
+  </si>
+  <si>
+    <t>432 PCS/</t>
+  </si>
+  <si>
+    <t>9,735 tn</t>
+  </si>
+  <si>
+    <t>34 247,50 USD</t>
+  </si>
+  <si>
+    <t>432 шт/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9,735 тн </t>
+  </si>
+  <si>
+    <t>34 247,50 $</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROOM 1105, NOBLIAN 2, 80, JUNGANG-DAERO, JUNG-GU, BUSAN, KOREA </t>
+  </si>
+  <si>
+    <t>*  f/v "Morskoy Volk"
+    MSC Frozen Alaska Pollock Roe - 222,021 tn (net weight)</t>
   </si>
   <si>
     <t>2) RONGCHENG KANGBAO AQUATIC FOODS CO., LTD.
@@ -712,89 +685,12 @@
     MSC Frozen Alaska Pollock Roe - 222,021 tn (net weight)</t>
   </si>
   <si>
-    <t>1) MARINE RENAISSANCE CO. LTD 
-ROOM 1105, NOBLIAN2, 80, JUNGANG-DAERO, JUNG-GU, BUSAN, KOREA
-* МФТ "Морской Волк"
-   MSC Молоки минтая мороженые - 9,585 тн (нетто)
-*  СРТМ "Си Хантер"
-    MSC Икра минтая - 0,150 тн (нетто)</t>
-  </si>
-  <si>
     <t>2) RONGCHENG KANGBAO AQUATIC FOODS CO., LTD.
 NO.189 XUNSHAN ROAD, XUNSHAN STREET, RONGCHENG, WEIHAI, SHANDONG PROVINCE	
 *  МФТ "Морской Волк"
     MSC Молоки минтая мороженые - 29,585 тн (нетто)
 *  МФТ "Морской Волк"
     MSC Икра минтая - 222,021 тн (нетто)</t>
-  </si>
-  <si>
-    <t>*  f/v "Sea Hunter"
-    MSC Frozen Alaska Pollock Roe
-    - USD 4 500,00 for one tn net weight</t>
-  </si>
-  <si>
-    <t>*  СРТМ "Си Хантер"
-    MSC Икра минтая
-    - 4 500,00 долл. за одну тонну (нетто)</t>
-  </si>
-  <si>
-    <t>*  СРТМ "Си Хантер"
-    MSC Икра минтая 
-    - 4 500,00 долл. за одну тонну (нетто)</t>
-  </si>
-  <si>
-    <t>FRSH-33T</t>
-  </si>
-  <si>
-    <t>MSC Frozen Alaska Pollock Roe</t>
-  </si>
-  <si>
-    <t>0,150 tn</t>
-  </si>
-  <si>
-    <t>4 500,00 USD</t>
-  </si>
-  <si>
-    <t>700,00 USD</t>
-  </si>
-  <si>
-    <t>6 PCS /</t>
-  </si>
-  <si>
-    <t>432 PCS/</t>
-  </si>
-  <si>
-    <t>9,735 tn</t>
-  </si>
-  <si>
-    <t>34 247,50 USD</t>
-  </si>
-  <si>
-    <t>432 шт/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9,735 тн </t>
-  </si>
-  <si>
-    <t>34 247,50 $</t>
-  </si>
-  <si>
-    <t>MSC Икра Минтая</t>
-  </si>
-  <si>
-    <t>6 шт /</t>
-  </si>
-  <si>
-    <t>0,150 тн</t>
-  </si>
-  <si>
-    <t>4 500,00 $</t>
-  </si>
-  <si>
-    <t>700,00 $</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROOM 1105, NOBLIAN 2, 80, JUNGANG-DAERO, JUNG-GU, BUSAN, KOREA </t>
   </si>
 </sst>
 </file>
@@ -1077,7 +973,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1423,6 +1319,18 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1742,10 +1650,10 @@
     <tabColor theme="9" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W86"/>
+  <dimension ref="A1:W90"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A29" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="140" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1773,7 +1681,7 @@
     <col min="24" max="24" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:22" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="14" t="s">
         <v>148</v>
       </c>
@@ -1794,7 +1702,7 @@
       <c r="Q1"/>
       <c r="R1"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:22" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="16" t="s">
         <v>24</v>
       </c>
@@ -1815,7 +1723,7 @@
       <c r="Q2"/>
       <c r="R2"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:22" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="16" t="s">
         <v>139</v>
       </c>
@@ -1840,32 +1748,20 @@
       <c r="U3" s="9"/>
       <c r="V3" s="9"/>
     </row>
-    <row r="4" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="18" t="s">
+    <row r="4" spans="1:22" s="124" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="125" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="126" t="s">
         <v>92</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
-    </row>
-    <row r="5" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+    </row>
+    <row r="5" spans="1:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="20" t="s">
         <v>93</v>
       </c>
@@ -1886,7 +1782,7 @@
       <c r="Q5"/>
       <c r="R5"/>
     </row>
-    <row r="6" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="22" t="s">
         <v>140</v>
       </c>
@@ -1906,7 +1802,7 @@
       <c r="Q6"/>
       <c r="R6"/>
     </row>
-    <row r="7" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="18" t="s">
         <v>152</v>
       </c>
@@ -1914,7 +1810,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="18" t="s">
         <v>141</v>
       </c>
@@ -1922,7 +1818,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="18" t="s">
         <v>142</v>
       </c>
@@ -1947,7 +1843,7 @@
       <c r="U9" s="11"/>
       <c r="V9" s="11"/>
     </row>
-    <row r="10" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
         <v>97</v>
       </c>
@@ -1967,7 +1863,7 @@
       <c r="Q10"/>
       <c r="R10"/>
     </row>
-    <row r="11" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:22" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="22" t="s">
         <v>12</v>
       </c>
@@ -1987,7 +1883,7 @@
       <c r="Q11"/>
       <c r="R11"/>
     </row>
-    <row r="12" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:22" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="18" t="s">
         <v>14</v>
       </c>
@@ -1995,7 +1891,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="18" t="s">
         <v>143</v>
       </c>
@@ -2003,7 +1899,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:22" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="18" t="s">
         <v>100</v>
       </c>
@@ -2011,7 +1907,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="24" t="s">
         <v>102</v>
       </c>
@@ -2019,7 +1915,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:22" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="18" t="s">
         <v>150</v>
       </c>
@@ -2044,12 +1940,12 @@
       <c r="U16"/>
       <c r="V16"/>
     </row>
-    <row r="17" spans="1:22" ht="33.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:22" ht="36.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="18" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F17"/>
       <c r="G17"/>
@@ -2069,13 +1965,9 @@
       <c r="U17"/>
       <c r="V17"/>
     </row>
-    <row r="18" spans="1:22" ht="33.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>167</v>
-      </c>
+    <row r="18" spans="1:22" ht="10.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="18"/>
+      <c r="B18" s="19"/>
       <c r="F18"/>
       <c r="G18"/>
       <c r="H18"/>
@@ -2094,12 +1986,12 @@
       <c r="U18"/>
       <c r="V18"/>
     </row>
-    <row r="19" spans="1:22" ht="33.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>169</v>
+    <row r="19" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>106</v>
       </c>
       <c r="F19"/>
       <c r="G19"/>
@@ -2119,12 +2011,12 @@
       <c r="U19"/>
       <c r="V19"/>
     </row>
-    <row r="20" spans="1:22" ht="33.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:22" ht="25.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="18" t="s">
-        <v>170</v>
+        <v>107</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="F20"/>
       <c r="G20"/>
@@ -2144,394 +2036,322 @@
       <c r="U20"/>
       <c r="V20"/>
     </row>
-    <row r="21" spans="1:22" ht="10.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="18"/>
-      <c r="B21" s="19"/>
-      <c r="F21"/>
-      <c r="G21"/>
-      <c r="H21"/>
-      <c r="I21"/>
-      <c r="J21"/>
-      <c r="K21"/>
-      <c r="L21"/>
-      <c r="M21"/>
-      <c r="N21"/>
-      <c r="O21"/>
-      <c r="P21"/>
-      <c r="Q21"/>
-      <c r="R21"/>
-      <c r="S21"/>
-      <c r="T21"/>
-      <c r="U21"/>
-      <c r="V21"/>
-    </row>
-    <row r="22" spans="1:22" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22"/>
-      <c r="I22"/>
-      <c r="J22"/>
-      <c r="K22"/>
-      <c r="L22"/>
-      <c r="M22"/>
-      <c r="N22"/>
-      <c r="O22"/>
-      <c r="P22"/>
-      <c r="Q22"/>
-      <c r="R22"/>
-      <c r="S22"/>
-      <c r="T22"/>
-      <c r="U22"/>
-      <c r="V22"/>
-    </row>
-    <row r="23" spans="1:22" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="F23"/>
-      <c r="G23"/>
-      <c r="H23"/>
-      <c r="I23"/>
-      <c r="J23"/>
-      <c r="K23"/>
-      <c r="L23"/>
-      <c r="M23"/>
-      <c r="N23"/>
-      <c r="O23"/>
-      <c r="P23"/>
-      <c r="Q23"/>
-      <c r="R23"/>
-      <c r="S23"/>
-      <c r="T23"/>
-      <c r="U23"/>
-      <c r="V23"/>
-    </row>
-    <row r="24" spans="1:22" ht="49.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="B24" s="27" t="s">
-        <v>172</v>
-      </c>
-      <c r="F24"/>
-      <c r="G24"/>
-      <c r="H24"/>
-      <c r="I24"/>
-      <c r="J24"/>
-      <c r="K24"/>
-      <c r="L24"/>
-      <c r="M24"/>
-      <c r="N24"/>
-      <c r="O24"/>
-      <c r="P24"/>
-      <c r="Q24"/>
-      <c r="R24"/>
-      <c r="S24"/>
-      <c r="T24"/>
-      <c r="U24"/>
-      <c r="V24"/>
-    </row>
-    <row r="25" spans="1:22" ht="49.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="26" t="s">
-        <v>177</v>
-      </c>
-      <c r="B25" s="27" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" ht="49.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="B26" s="27" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" ht="49.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="26" t="s">
-        <v>177</v>
-      </c>
-      <c r="B27" s="27" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" s="12" customFormat="1" ht="58.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="36" t="s">
+    <row r="21" spans="1:22" ht="49.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" s="12" customFormat="1" ht="54.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="B28" s="37" t="s">
+      <c r="B22" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="13"/>
-      <c r="R28" s="13"/>
-      <c r="S28" s="13"/>
-      <c r="T28" s="13"/>
-      <c r="U28" s="13"/>
-      <c r="V28" s="13"/>
-    </row>
-    <row r="29" spans="1:22" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="32" t="s">
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="13"/>
+      <c r="V22" s="13"/>
+    </row>
+    <row r="23" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="B29" s="32" t="s">
+      <c r="B23" s="32" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:22" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="18" t="s">
+    <row r="24" spans="1:22" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B24" s="19" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="18" t="s">
+    <row r="25" spans="1:22" ht="38.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="B25" s="19" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="32" spans="1:22" s="34" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="33" t="s">
+    <row r="26" spans="1:22" s="34" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="B32" s="33" t="s">
+      <c r="B26" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="F32" s="35"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="35"/>
-      <c r="J32" s="35"/>
-      <c r="K32" s="35"/>
-      <c r="L32" s="35"/>
-      <c r="M32" s="35"/>
-      <c r="N32" s="35"/>
-      <c r="O32" s="35"/>
-      <c r="P32" s="35"/>
-      <c r="Q32" s="35"/>
-      <c r="R32" s="35"/>
-      <c r="S32" s="35"/>
-      <c r="T32" s="35"/>
-      <c r="U32" s="35"/>
-      <c r="V32" s="35"/>
-    </row>
-    <row r="33" spans="1:2" ht="131.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="35"/>
+      <c r="M26" s="35"/>
+      <c r="N26" s="35"/>
+      <c r="O26" s="35"/>
+      <c r="P26" s="35"/>
+      <c r="Q26" s="35"/>
+      <c r="R26" s="35"/>
+      <c r="S26" s="35"/>
+      <c r="T26" s="35"/>
+      <c r="U26" s="35"/>
+      <c r="V26" s="35"/>
+    </row>
+    <row r="27" spans="1:22" ht="124.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="18" t="s">
-        <v>173</v>
+        <v>9</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="131.75" customHeight="1" x14ac:dyDescent="0.45">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="18" t="s">
-        <v>174</v>
+        <v>124</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="B35" s="25" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="18" t="s">
-        <v>119</v>
+        <v>53</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="B37" s="25" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="B38" s="23" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A38" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="22" t="s">
-        <v>5</v>
+        <v>97</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B40" s="19" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="25.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="18" t="s">
-        <v>124</v>
+        <v>14</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="18" t="s">
-        <v>52</v>
+        <v>129</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="18" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="18" t="s">
-        <v>54</v>
+        <v>131</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="18" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="B46" s="23" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B47" s="23" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B48" s="19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="B49" s="19" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="B50" s="19" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="B51" s="19" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="B52" s="19" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="18" t="s">
+    </row>
+    <row r="46" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="B53" s="19" t="s">
+      <c r="B46" s="19" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="13.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="28" t="s">
+    <row r="47" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="B54" s="29" t="s">
+      <c r="B47" s="29" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="30" t="s">
+    <row r="48" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="B55" s="30" t="s">
+      <c r="B48" s="30" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="57" spans="1:2" ht="13.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="58" spans="1:2" ht="38.65" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="59" spans="1:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="60" spans="1:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="61" spans="1:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="62" spans="1:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="64" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="79" ht="26.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="86" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="49" spans="1:2" ht="10.9" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="127"/>
+      <c r="B49" s="127"/>
+    </row>
+    <row r="50" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="127"/>
+      <c r="B50" s="127"/>
+    </row>
+    <row r="51" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="127"/>
+      <c r="B51" s="127"/>
+    </row>
+    <row r="52" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A52" s="127"/>
+      <c r="B52" s="127"/>
+    </row>
+    <row r="53" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A53" s="127"/>
+      <c r="B53" s="127"/>
+    </row>
+    <row r="54" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A54" s="127"/>
+      <c r="B54" s="127"/>
+    </row>
+    <row r="55" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A55" s="127"/>
+      <c r="B55" s="127"/>
+    </row>
+    <row r="56" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A56" s="127"/>
+      <c r="B56" s="127"/>
+    </row>
+    <row r="57" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A57" s="127"/>
+      <c r="B57" s="127"/>
+    </row>
+    <row r="58" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A58" s="127"/>
+      <c r="B58" s="127"/>
+    </row>
+    <row r="59" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A59" s="127"/>
+      <c r="B59" s="127"/>
+    </row>
+    <row r="60" spans="1:2" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="61" spans="1:2" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="62" spans="1:2" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="63" spans="1:2" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="64" spans="1:2" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="65" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="66" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="67" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="68" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="69" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="70" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="71" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="83" ht="26.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="90" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{13E4E285-FA5D-41CC-AC7F-578EA8AF8279}">
@@ -2545,11 +2365,8 @@
   <pageMargins left="0.31496062992125984" right="0.11811023622047245" top="0.15748031496062992" bottom="0.15748031496062992" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="91" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="28" max="16383" man="1"/>
+    <brk id="22" max="16383" man="1"/>
   </rowBreaks>
-  <colBreaks count="1" manualBreakCount="1">
-    <brk id="2" max="1048575" man="1"/>
-  </colBreaks>
 </worksheet>
 </file>
 
@@ -2559,10 +2376,10 @@
     <tabColor theme="9" tint="-0.499984740745262"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:AA114"/>
+  <dimension ref="A2:AA112"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A83" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81:H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2686,7 +2503,7 @@
     </row>
     <row r="8" spans="1:27" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="109" t="s">
-        <v>197</v>
+        <v>168</v>
       </c>
       <c r="B8" s="110"/>
       <c r="C8" s="110"/>
@@ -2761,7 +2578,7 @@
     </row>
     <row r="13" spans="1:27" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="51" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D13" s="66"/>
       <c r="E13" s="53" t="s">
@@ -2861,31 +2678,15 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="42" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="49" t="s">
-        <v>180</v>
-      </c>
-      <c r="B17" s="74" t="s">
-        <v>163</v>
-      </c>
-      <c r="C17" s="74" t="s">
-        <v>181</v>
-      </c>
-      <c r="D17" s="74" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="74" t="s">
-        <v>185</v>
-      </c>
-      <c r="F17" s="74" t="s">
-        <v>182</v>
-      </c>
-      <c r="G17" s="74" t="s">
-        <v>183</v>
-      </c>
-      <c r="H17" s="50" t="s">
-        <v>184</v>
-      </c>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A17" s="49"/>
+      <c r="B17" s="74"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="74"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="74"/>
+      <c r="H17" s="50"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A18" s="49"/>
@@ -2906,6 +2707,27 @@
       <c r="F19" s="74"/>
       <c r="G19" s="74"/>
       <c r="H19" s="50"/>
+      <c r="R19" t="s">
+        <v>35</v>
+      </c>
+      <c r="S19" t="s">
+        <v>37</v>
+      </c>
+      <c r="T19">
+        <v>22.500000000000004</v>
+      </c>
+      <c r="U19">
+        <v>426</v>
+      </c>
+      <c r="V19">
+        <v>9.5850000000000009</v>
+      </c>
+      <c r="W19">
+        <v>3500</v>
+      </c>
+      <c r="X19">
+        <v>33547.5</v>
+      </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A20" s="49"/>
@@ -2916,27 +2738,6 @@
       <c r="F20" s="74"/>
       <c r="G20" s="74"/>
       <c r="H20" s="50"/>
-      <c r="R20" t="s">
-        <v>35</v>
-      </c>
-      <c r="S20" t="s">
-        <v>37</v>
-      </c>
-      <c r="T20">
-        <v>22.500000000000004</v>
-      </c>
-      <c r="U20">
-        <v>426</v>
-      </c>
-      <c r="V20">
-        <v>9.5850000000000009</v>
-      </c>
-      <c r="W20">
-        <v>3500</v>
-      </c>
-      <c r="X20">
-        <v>33547.5</v>
-      </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A21" s="49"/>
@@ -3037,6 +2838,9 @@
       <c r="F30" s="74"/>
       <c r="G30" s="74"/>
       <c r="H30" s="50"/>
+      <c r="R30">
+        <v>33547.5</v>
+      </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A31" s="49"/>
@@ -3047,9 +2851,6 @@
       <c r="F31" s="74"/>
       <c r="G31" s="74"/>
       <c r="H31" s="50"/>
-      <c r="R31">
-        <v>33547.5</v>
-      </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A32" s="49"/>
@@ -3118,21 +2919,23 @@
       <c r="D38" s="74"/>
       <c r="E38" s="74"/>
       <c r="F38" s="74"/>
-      <c r="G38" s="74"/>
-      <c r="H38" s="50"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A39" s="49"/>
-      <c r="B39" s="74"/>
-      <c r="C39" s="74"/>
-      <c r="D39" s="74"/>
-      <c r="E39" s="74"/>
-      <c r="F39" s="74"/>
-      <c r="G39" s="75"/>
-      <c r="H39" s="76"/>
-    </row>
-    <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="2"/>
+      <c r="G38" s="75"/>
+      <c r="H38" s="76"/>
+    </row>
+    <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="2"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -3142,75 +2945,73 @@
       <c r="H40" s="4"/>
     </row>
     <row r="41" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="4"/>
-    </row>
-    <row r="42" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="77" t="s">
+      <c r="A41" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="78"/>
-      <c r="C42" s="78"/>
-      <c r="D42" s="78"/>
-      <c r="E42" s="78"/>
-      <c r="F42" s="78"/>
-      <c r="G42" s="78"/>
-      <c r="H42" s="79"/>
+      <c r="B41" s="78"/>
+      <c r="C41" s="78"/>
+      <c r="D41" s="78"/>
+      <c r="E41" s="78"/>
+      <c r="F41" s="78"/>
+      <c r="G41" s="78"/>
+      <c r="H41" s="79"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A42" s="61"/>
+      <c r="B42" s="40"/>
+      <c r="C42" s="80" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="80" t="s">
+        <v>162</v>
+      </c>
+      <c r="E42" s="81" t="s">
+        <v>163</v>
+      </c>
+      <c r="G42" s="82"/>
+      <c r="H42" s="83" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A43" s="61"/>
-      <c r="B43" s="40"/>
-      <c r="C43" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="D43" s="80" t="s">
-        <v>186</v>
-      </c>
-      <c r="E43" s="81" t="s">
-        <v>187</v>
-      </c>
+      <c r="A43" s="119" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="120"/>
+      <c r="C43" s="120"/>
+      <c r="D43" s="120"/>
+      <c r="E43" s="120"/>
+      <c r="F43" s="120"/>
       <c r="G43" s="82"/>
-      <c r="H43" s="83" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A44" s="119" t="s">
-        <v>49</v>
-      </c>
-      <c r="B44" s="120"/>
-      <c r="C44" s="120"/>
-      <c r="D44" s="120"/>
-      <c r="E44" s="120"/>
-      <c r="F44" s="120"/>
-      <c r="G44" s="82"/>
-      <c r="H44" s="66"/>
-    </row>
-    <row r="45" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="84" t="s">
+      <c r="H43" s="66"/>
+    </row>
+    <row r="44" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="85"/>
-      <c r="C45" s="85"/>
-      <c r="D45" s="85"/>
-      <c r="E45" s="53" t="s">
+      <c r="B44" s="85"/>
+      <c r="C44" s="85"/>
+      <c r="D44" s="85"/>
+      <c r="E44" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="F45" s="54"/>
-      <c r="G45" s="54"/>
-      <c r="H45" s="56"/>
-    </row>
-    <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F44" s="54"/>
+      <c r="G44" s="54"/>
+      <c r="H44" s="56"/>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" s="48"/>
+      <c r="C45" s="48"/>
+      <c r="D45" s="48"/>
+      <c r="E45" s="51"/>
+      <c r="H45" s="52"/>
+    </row>
+    <row r="46" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="47" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B46" s="48"/>
       <c r="C46" s="48"/>
@@ -3218,9 +3019,9 @@
       <c r="E46" s="51"/>
       <c r="H46" s="52"/>
     </row>
-    <row r="47" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="47" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B47" s="48"/>
       <c r="C47" s="48"/>
@@ -3228,113 +3029,109 @@
       <c r="E47" s="51"/>
       <c r="H47" s="52"/>
     </row>
-    <row r="48" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="B48" s="48"/>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="51"/>
-      <c r="H48" s="52"/>
-    </row>
-    <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="71" t="s">
+    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="B49" s="72"/>
-      <c r="C49" s="72"/>
-      <c r="D49" s="73"/>
-      <c r="E49" s="86"/>
-      <c r="F49" s="69"/>
-      <c r="G49" s="69"/>
-      <c r="H49" s="70"/>
-    </row>
-    <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B48" s="72"/>
+      <c r="C48" s="72"/>
+      <c r="D48" s="73"/>
+      <c r="E48" s="86"/>
+      <c r="F48" s="69"/>
+      <c r="G48" s="69"/>
+      <c r="H48" s="70"/>
+    </row>
+    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="45"/>
+      <c r="B49" s="45"/>
+      <c r="C49" s="45"/>
+      <c r="D49" s="45"/>
+    </row>
+    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="45"/>
       <c r="B50" s="45"/>
       <c r="C50" s="45"/>
       <c r="D50" s="45"/>
     </row>
-    <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="45"/>
       <c r="B51" s="45"/>
       <c r="C51" s="45"/>
       <c r="D51" s="45"/>
     </row>
-    <row r="52" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="45"/>
       <c r="B52" s="45"/>
       <c r="C52" s="45"/>
       <c r="D52" s="45"/>
     </row>
-    <row r="53" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="45"/>
       <c r="B53" s="45"/>
       <c r="C53" s="45"/>
       <c r="D53" s="45"/>
     </row>
-    <row r="54" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="45"/>
       <c r="B54" s="45"/>
       <c r="C54" s="45"/>
       <c r="D54" s="45"/>
     </row>
-    <row r="55" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="45"/>
       <c r="B55" s="45"/>
       <c r="C55" s="45"/>
       <c r="D55" s="45"/>
     </row>
-    <row r="56" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="45"/>
       <c r="B56" s="45"/>
       <c r="C56" s="45"/>
       <c r="D56" s="45"/>
     </row>
-    <row r="57" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="45"/>
       <c r="B57" s="45"/>
       <c r="C57" s="45"/>
       <c r="D57" s="45"/>
     </row>
-    <row r="58" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="45"/>
       <c r="B58" s="45"/>
       <c r="C58" s="45"/>
       <c r="D58" s="45"/>
     </row>
-    <row r="59" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="45"/>
       <c r="B59" s="45"/>
       <c r="C59" s="45"/>
       <c r="D59" s="45"/>
     </row>
-    <row r="60" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="45"/>
       <c r="B60" s="45"/>
       <c r="C60" s="45"/>
       <c r="D60" s="45"/>
     </row>
-    <row r="61" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="45"/>
       <c r="B61" s="45"/>
       <c r="C61" s="45"/>
       <c r="D61" s="45"/>
     </row>
-    <row r="62" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62" s="45"/>
       <c r="B62" s="45"/>
       <c r="C62" s="45"/>
       <c r="D62" s="45"/>
     </row>
-    <row r="63" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="45"/>
       <c r="B63" s="45"/>
       <c r="C63" s="45"/>
       <c r="D63" s="45"/>
     </row>
-    <row r="64" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="45"/>
       <c r="B64" s="45"/>
       <c r="C64" s="45"/>
@@ -3352,275 +3149,263 @@
       <c r="C66" s="45"/>
       <c r="D66" s="45"/>
     </row>
-    <row r="67" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A67" s="45"/>
-      <c r="B67" s="45"/>
-      <c r="C67" s="45"/>
-      <c r="D67" s="45"/>
-    </row>
-    <row r="68" spans="1:8" ht="28.15" customHeight="1" x14ac:dyDescent="0.85">
-      <c r="A68" s="107" t="s">
+    <row r="67" spans="1:8" ht="28.15" customHeight="1" x14ac:dyDescent="0.85">
+      <c r="A67" s="107" t="s">
         <v>56</v>
       </c>
-      <c r="B68" s="87"/>
-      <c r="C68" s="87"/>
-      <c r="D68" s="87"/>
-      <c r="E68" s="87"/>
-      <c r="F68" s="87"/>
-      <c r="G68" s="87"/>
-      <c r="H68" s="87"/>
+      <c r="B67" s="87"/>
+      <c r="C67" s="87"/>
+      <c r="D67" s="87"/>
+      <c r="E67" s="87"/>
+      <c r="F67" s="87"/>
+      <c r="G67" s="87"/>
+      <c r="H67" s="87"/>
+    </row>
+    <row r="68" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A68" s="88" t="s">
+        <v>57</v>
+      </c>
+      <c r="B68" s="89"/>
+      <c r="C68" s="89"/>
+      <c r="D68" s="89"/>
+      <c r="E68" s="88" t="s">
+        <v>58</v>
+      </c>
+      <c r="F68" s="89"/>
+      <c r="G68" s="90" t="s">
+        <v>3</v>
+      </c>
+      <c r="H68" s="91" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="69" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A69" s="88" t="s">
-        <v>57</v>
-      </c>
-      <c r="B69" s="89"/>
-      <c r="C69" s="89"/>
-      <c r="D69" s="89"/>
-      <c r="E69" s="88" t="s">
-        <v>58</v>
-      </c>
-      <c r="F69" s="89"/>
-      <c r="G69" s="90" t="s">
-        <v>3</v>
-      </c>
-      <c r="H69" s="91" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A70" s="59" t="s">
+      <c r="A69" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="B70" s="45"/>
-      <c r="C70" s="45"/>
+      <c r="B69" s="45"/>
+      <c r="C69" s="45"/>
+      <c r="D69" s="45"/>
+      <c r="E69" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="F69" s="48"/>
+      <c r="G69" s="92" t="s">
+        <v>7</v>
+      </c>
+      <c r="H69" s="76" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A70" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="B70" s="72"/>
+      <c r="C70" s="72"/>
       <c r="D70" s="45"/>
-      <c r="E70" s="47" t="s">
-        <v>60</v>
-      </c>
-      <c r="F70" s="48"/>
-      <c r="G70" s="92" t="s">
-        <v>7</v>
-      </c>
-      <c r="H70" s="76" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A71" s="71" t="s">
-        <v>61</v>
-      </c>
-      <c r="B71" s="72"/>
-      <c r="C71" s="72"/>
-      <c r="D71" s="45"/>
-      <c r="E71" s="59"/>
-      <c r="F71" s="45"/>
-      <c r="G71" s="51"/>
-      <c r="H71" s="52"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A72" s="93" t="s">
+      <c r="E70" s="59"/>
+      <c r="F70" s="45"/>
+      <c r="G70" s="51"/>
+      <c r="H70" s="52"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A71" s="93" t="s">
         <v>62</v>
       </c>
-      <c r="B72" s="89"/>
-      <c r="C72" s="89"/>
-      <c r="D72" s="94"/>
-      <c r="E72" s="53" t="s">
+      <c r="B71" s="89"/>
+      <c r="C71" s="89"/>
+      <c r="D71" s="94"/>
+      <c r="E71" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="F72" s="54"/>
-      <c r="G72" s="54"/>
-      <c r="H72" s="56"/>
-    </row>
-    <row r="73" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A73" s="47" t="s">
+      <c r="F71" s="54"/>
+      <c r="G71" s="54"/>
+      <c r="H71" s="56"/>
+    </row>
+    <row r="72" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A72" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B73" s="48"/>
-      <c r="C73" s="48"/>
-      <c r="D73" s="48"/>
-      <c r="E73" s="59" t="s">
+      <c r="B72" s="48"/>
+      <c r="C72" s="48"/>
+      <c r="D72" s="48"/>
+      <c r="E72" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="F73" s="45"/>
-      <c r="G73" s="45"/>
-      <c r="H73" s="60"/>
-    </row>
-    <row r="74" spans="1:8" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A74" s="112" t="s">
+      <c r="F72" s="45"/>
+      <c r="G72" s="45"/>
+      <c r="H72" s="60"/>
+    </row>
+    <row r="73" spans="1:8" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A73" s="112" t="s">
         <v>15</v>
       </c>
-      <c r="B74" s="113"/>
-      <c r="C74" s="113"/>
-      <c r="D74" s="114"/>
-      <c r="E74" s="112" t="s">
+      <c r="B73" s="113"/>
+      <c r="C73" s="113"/>
+      <c r="D73" s="114"/>
+      <c r="E73" s="112" t="s">
         <v>146</v>
       </c>
-      <c r="F74" s="113"/>
-      <c r="G74" s="113"/>
-      <c r="H74" s="114"/>
+      <c r="F73" s="113"/>
+      <c r="G73" s="113"/>
+      <c r="H73" s="114"/>
+    </row>
+    <row r="74" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A74" s="95" t="s">
+        <v>64</v>
+      </c>
+      <c r="B74" s="64" t="s">
+        <v>156</v>
+      </c>
+      <c r="D74" s="52"/>
+      <c r="E74" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="F74" s="54"/>
+      <c r="G74" s="54"/>
+      <c r="H74" s="56"/>
     </row>
     <row r="75" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A75" s="95" t="s">
-        <v>64</v>
-      </c>
-      <c r="B75" s="64" t="s">
-        <v>160</v>
+      <c r="A75" s="59" t="s">
+        <v>66</v>
+      </c>
+      <c r="B75" s="96" t="s">
+        <v>67</v>
       </c>
       <c r="D75" s="52"/>
-      <c r="E75" s="53" t="s">
-        <v>65</v>
-      </c>
-      <c r="F75" s="54"/>
-      <c r="G75" s="54"/>
-      <c r="H75" s="56"/>
-    </row>
-    <row r="76" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A76" s="59" t="s">
-        <v>66</v>
-      </c>
-      <c r="B76" s="96" t="s">
-        <v>67</v>
-      </c>
-      <c r="D76" s="52"/>
-      <c r="E76" s="39" t="s">
+      <c r="E75" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="F76" s="64"/>
-      <c r="G76" s="64"/>
-      <c r="H76" s="65"/>
-    </row>
-    <row r="77" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A77" s="95" t="s">
+      <c r="F75" s="64"/>
+      <c r="G75" s="64"/>
+      <c r="H75" s="65"/>
+    </row>
+    <row r="76" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A76" s="95" t="s">
         <v>69</v>
       </c>
-      <c r="B77" s="97" t="s">
+      <c r="B76" s="97" t="s">
         <v>70</v>
       </c>
-      <c r="D77" s="66"/>
-      <c r="E77" s="59" t="s">
+      <c r="D76" s="66"/>
+      <c r="E76" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="F77" s="45"/>
-      <c r="G77" s="45"/>
-      <c r="H77" s="60"/>
-    </row>
-    <row r="78" spans="1:8" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A78" s="67" t="s">
-        <v>159</v>
-      </c>
-      <c r="B78" s="72" t="s">
+      <c r="F76" s="45"/>
+      <c r="G76" s="45"/>
+      <c r="H76" s="60"/>
+    </row>
+    <row r="77" spans="1:8" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A77" s="67" t="s">
+        <v>155</v>
+      </c>
+      <c r="B77" s="72" t="s">
         <v>72</v>
       </c>
-      <c r="D78" s="70"/>
-      <c r="E78" s="71" t="s">
+      <c r="D77" s="70"/>
+      <c r="E77" s="71" t="s">
         <v>73</v>
       </c>
-      <c r="F78" s="72"/>
-      <c r="G78" s="72"/>
-      <c r="H78" s="73"/>
-    </row>
-    <row r="79" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A79" s="51" t="s">
-        <v>158</v>
-      </c>
-      <c r="C79" s="98"/>
-      <c r="D79" s="66"/>
-      <c r="E79" s="53" t="s">
+      <c r="F77" s="72"/>
+      <c r="G77" s="72"/>
+      <c r="H77" s="73"/>
+    </row>
+    <row r="78" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A78" s="51" t="s">
+        <v>154</v>
+      </c>
+      <c r="C78" s="98"/>
+      <c r="D78" s="66"/>
+      <c r="E78" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="F79" s="54"/>
-      <c r="G79" s="54"/>
-      <c r="H79" s="56"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A80" s="51"/>
-      <c r="C80" s="69"/>
-      <c r="D80" s="99"/>
-      <c r="E80" s="71" t="s">
+      <c r="F78" s="54"/>
+      <c r="G78" s="54"/>
+      <c r="H78" s="56"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A79" s="51"/>
+      <c r="C79" s="69"/>
+      <c r="D79" s="99"/>
+      <c r="E79" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="F80" s="72"/>
-      <c r="G80" s="72"/>
-      <c r="H80" s="73"/>
-    </row>
-    <row r="81" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A81" s="100" t="s">
+      <c r="F79" s="72"/>
+      <c r="G79" s="72"/>
+      <c r="H79" s="73"/>
+    </row>
+    <row r="80" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A80" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="B81" s="101" t="s">
-        <v>161</v>
-      </c>
-      <c r="C81" s="101" t="s">
+      <c r="B80" s="101" t="s">
+        <v>157</v>
+      </c>
+      <c r="C80" s="101" t="s">
         <v>76</v>
       </c>
-      <c r="D81" s="101" t="s">
+      <c r="D80" s="101" t="s">
         <v>77</v>
       </c>
-      <c r="E81" s="102" t="s">
+      <c r="E80" s="102" t="s">
         <v>78</v>
       </c>
-      <c r="F81" s="102"/>
-      <c r="G81" s="101" t="s">
+      <c r="F80" s="102"/>
+      <c r="G80" s="101" t="s">
         <v>79</v>
       </c>
-      <c r="H81" s="103" t="s">
+      <c r="H80" s="103" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:17" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A82" s="49" t="s">
+    <row r="81" spans="1:17" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A81" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="B82" s="74" t="s">
+      <c r="B81" s="74" t="s">
         <v>86</v>
       </c>
-      <c r="C82" s="74" t="s">
+      <c r="C81" s="74" t="s">
         <v>104</v>
       </c>
-      <c r="D82" s="74" t="s">
+      <c r="D81" s="74" t="s">
         <v>81</v>
       </c>
-      <c r="E82" s="74" t="s">
+      <c r="E81" s="74" t="s">
         <v>82</v>
       </c>
-      <c r="F82" s="74" t="s">
+      <c r="F81" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="G82" s="74" t="s">
+      <c r="G81" s="74" t="s">
         <v>84</v>
       </c>
-      <c r="H82" s="50" t="s">
+      <c r="H81" s="50" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="83" spans="1:17" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A83" s="49" t="s">
-        <v>180</v>
-      </c>
-      <c r="B83" s="74" t="s">
-        <v>162</v>
-      </c>
-      <c r="C83" s="74" t="s">
-        <v>192</v>
-      </c>
-      <c r="D83" s="74" t="s">
-        <v>81</v>
-      </c>
-      <c r="E83" s="74" t="s">
-        <v>193</v>
-      </c>
-      <c r="F83" s="74" t="s">
-        <v>194</v>
-      </c>
-      <c r="G83" s="74" t="s">
-        <v>195</v>
-      </c>
-      <c r="H83" s="50" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="84" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A82" s="49"/>
+      <c r="B82" s="74"/>
+      <c r="C82" s="74"/>
+      <c r="D82" s="74"/>
+      <c r="E82" s="74"/>
+      <c r="F82" s="74"/>
+      <c r="G82" s="74"/>
+      <c r="H82" s="50"/>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A83" s="49"/>
+      <c r="B83" s="74"/>
+      <c r="C83" s="74"/>
+      <c r="D83" s="74"/>
+      <c r="E83" s="74"/>
+      <c r="F83" s="74"/>
+      <c r="G83" s="74"/>
+      <c r="H83" s="50"/>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A84" s="49"/>
       <c r="B84" s="74"/>
       <c r="C84" s="74"/>
@@ -3631,11 +3416,6 @@
       <c r="H84" s="50"/>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A85" s="49"/>
-      <c r="B85" s="74"/>
-      <c r="C85" s="74"/>
-      <c r="D85" s="74"/>
-      <c r="E85" s="74"/>
       <c r="F85" s="74"/>
       <c r="G85" s="74"/>
       <c r="H85" s="50"/>
@@ -3649,8 +3429,14 @@
       <c r="F86" s="74"/>
       <c r="G86" s="74"/>
       <c r="H86" s="50"/>
+      <c r="Q86" s="104"/>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A87" s="49"/>
+      <c r="B87" s="74"/>
+      <c r="C87" s="74"/>
+      <c r="D87" s="74"/>
+      <c r="E87" s="74"/>
       <c r="F87" s="74"/>
       <c r="G87" s="74"/>
       <c r="H87" s="50"/>
@@ -3664,7 +3450,6 @@
       <c r="F88" s="74"/>
       <c r="G88" s="74"/>
       <c r="H88" s="50"/>
-      <c r="Q88" s="104"/>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A89" s="49"/>
@@ -3752,7 +3537,6 @@
       <c r="C97" s="74"/>
       <c r="D97" s="74"/>
       <c r="E97" s="74"/>
-      <c r="F97" s="74"/>
       <c r="G97" s="74"/>
       <c r="H97" s="50"/>
     </row>
@@ -3772,6 +3556,7 @@
       <c r="C99" s="74"/>
       <c r="D99" s="74"/>
       <c r="E99" s="74"/>
+      <c r="F99" s="74"/>
       <c r="G99" s="74"/>
       <c r="H99" s="50"/>
     </row>
@@ -3796,115 +3581,115 @@
       <c r="H101" s="50"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A102" s="49"/>
-      <c r="B102" s="74"/>
-      <c r="C102" s="74"/>
-      <c r="D102" s="74"/>
-      <c r="E102" s="74"/>
-      <c r="F102" s="74"/>
-      <c r="G102" s="74"/>
-      <c r="H102" s="50"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A103" s="49"/>
-      <c r="B103" s="74"/>
-      <c r="C103" s="74"/>
-      <c r="D103" s="74"/>
-      <c r="E103" s="74"/>
-      <c r="F103" s="74"/>
-      <c r="G103" s="74"/>
-      <c r="H103" s="50"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A104" s="62"/>
-      <c r="B104" s="46"/>
-      <c r="C104" s="46"/>
-      <c r="D104" s="46"/>
-      <c r="E104" s="46"/>
-      <c r="F104" s="46"/>
-      <c r="G104" s="82"/>
-      <c r="H104" s="66"/>
+      <c r="A102" s="62"/>
+      <c r="B102" s="46"/>
+      <c r="C102" s="46"/>
+      <c r="D102" s="46"/>
+      <c r="E102" s="46"/>
+      <c r="F102" s="46"/>
+      <c r="G102" s="82"/>
+      <c r="H102" s="66"/>
+    </row>
+    <row r="103" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A103" s="5"/>
+      <c r="B103" s="6"/>
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="6"/>
+      <c r="F103" s="6"/>
+      <c r="G103" s="6"/>
+      <c r="H103" s="7"/>
+    </row>
+    <row r="104" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A104" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B104" s="6"/>
+      <c r="C104" s="6"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="6"/>
+      <c r="F104" s="6"/>
+      <c r="G104" s="6"/>
+      <c r="H104" s="7"/>
     </row>
     <row r="105" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A105" s="5"/>
-      <c r="B105" s="6"/>
-      <c r="C105" s="6"/>
-      <c r="D105" s="6"/>
-      <c r="E105" s="6"/>
-      <c r="F105" s="6"/>
-      <c r="G105" s="6"/>
-      <c r="H105" s="7"/>
-    </row>
-    <row r="106" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A106" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="B106" s="6"/>
-      <c r="C106" s="6"/>
-      <c r="D106" s="6"/>
-      <c r="E106" s="6"/>
-      <c r="F106" s="6"/>
-      <c r="G106" s="6"/>
-      <c r="H106" s="7"/>
-    </row>
-    <row r="107" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A107" s="77" t="s">
+      <c r="A105" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="B107" s="78"/>
-      <c r="C107" s="78"/>
-      <c r="D107" s="78"/>
-      <c r="E107" s="78"/>
-      <c r="F107" s="78"/>
-      <c r="G107" s="78"/>
-      <c r="H107" s="79"/>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A108" s="61"/>
-      <c r="B108" s="40"/>
-      <c r="C108" s="80" t="s">
+      <c r="B105" s="78"/>
+      <c r="C105" s="78"/>
+      <c r="D105" s="78"/>
+      <c r="E105" s="78"/>
+      <c r="F105" s="78"/>
+      <c r="G105" s="78"/>
+      <c r="H105" s="79"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A106" s="61"/>
+      <c r="B106" s="40"/>
+      <c r="C106" s="80" t="s">
         <v>87</v>
       </c>
-      <c r="D108" s="80" t="s">
-        <v>189</v>
-      </c>
-      <c r="E108" s="105" t="s">
-        <v>190</v>
-      </c>
-      <c r="G108" s="82"/>
-      <c r="H108" s="83" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A109" s="119" t="s">
+      <c r="D106" s="80" t="s">
+        <v>165</v>
+      </c>
+      <c r="E106" s="105" t="s">
+        <v>166</v>
+      </c>
+      <c r="G106" s="82"/>
+      <c r="H106" s="83" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A107" s="119" t="s">
         <v>49</v>
       </c>
-      <c r="B109" s="120"/>
-      <c r="C109" s="120"/>
-      <c r="D109" s="120"/>
-      <c r="E109" s="120"/>
-      <c r="F109" s="120"/>
-      <c r="G109" s="82"/>
-      <c r="H109" s="66"/>
+      <c r="B107" s="120"/>
+      <c r="C107" s="120"/>
+      <c r="D107" s="120"/>
+      <c r="E107" s="120"/>
+      <c r="F107" s="120"/>
+      <c r="G107" s="82"/>
+      <c r="H107" s="66"/>
+    </row>
+    <row r="108" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A108" s="84" t="s">
+        <v>50</v>
+      </c>
+      <c r="B108" s="85"/>
+      <c r="C108" s="85"/>
+      <c r="D108" s="85"/>
+      <c r="E108" s="53" t="s">
+        <v>145</v>
+      </c>
+      <c r="F108" s="54"/>
+      <c r="G108" s="54"/>
+      <c r="H108" s="56"/>
+    </row>
+    <row r="109" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A109" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="B109" s="48"/>
+      <c r="C109" s="48"/>
+      <c r="D109" s="48"/>
+      <c r="E109" s="51"/>
+      <c r="H109" s="52"/>
     </row>
     <row r="110" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A110" s="84" t="s">
-        <v>50</v>
-      </c>
-      <c r="B110" s="85"/>
-      <c r="C110" s="85"/>
-      <c r="D110" s="85"/>
-      <c r="E110" s="53" t="s">
-        <v>145</v>
-      </c>
-      <c r="F110" s="54"/>
-      <c r="G110" s="54"/>
-      <c r="H110" s="56"/>
+      <c r="A110" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="B110" s="48"/>
+      <c r="C110" s="48"/>
+      <c r="D110" s="48"/>
+      <c r="E110" s="51"/>
+      <c r="H110" s="52"/>
     </row>
     <row r="111" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A111" s="47" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="B111" s="48"/>
       <c r="C111" s="48"/>
@@ -3913,36 +3698,16 @@
       <c r="H111" s="52"/>
     </row>
     <row r="112" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A112" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="B112" s="48"/>
-      <c r="C112" s="48"/>
-      <c r="D112" s="48"/>
-      <c r="E112" s="51"/>
-      <c r="H112" s="52"/>
-    </row>
-    <row r="113" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A113" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="B113" s="48"/>
-      <c r="C113" s="48"/>
-      <c r="D113" s="48"/>
-      <c r="E113" s="51"/>
-      <c r="H113" s="52"/>
-    </row>
-    <row r="114" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A114" s="71" t="s">
+      <c r="A112" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="B114" s="72"/>
-      <c r="C114" s="72"/>
-      <c r="D114" s="72"/>
-      <c r="E114" s="86"/>
-      <c r="F114" s="69"/>
-      <c r="G114" s="69"/>
-      <c r="H114" s="70"/>
+      <c r="B112" s="72"/>
+      <c r="C112" s="72"/>
+      <c r="D112" s="72"/>
+      <c r="E112" s="86"/>
+      <c r="F112" s="69"/>
+      <c r="G112" s="69"/>
+      <c r="H112" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -3950,10 +3715,10 @@
     <mergeCell ref="E8:H8"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A109:F109"/>
-    <mergeCell ref="A74:D74"/>
-    <mergeCell ref="E74:H74"/>
-    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A107:F107"/>
+    <mergeCell ref="A73:D73"/>
+    <mergeCell ref="E73:H73"/>
+    <mergeCell ref="A43:F43"/>
     <mergeCell ref="E14:H14"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
checkout, implementing storage template, generalizing contracts
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement_Vessels.xlsx
+++ b/templates/Export_Agreement_Vessels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD720957-086E-488C-BB32-256144E6A3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527C55F5-0C92-4D65-8A48-A46CF3D7A268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-55778" yWindow="-907" windowWidth="28995" windowHeight="15795" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Com_Invoice" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Export_Contract!$A$1:$B$70</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Export_Contract!$A$1:$B$65</definedName>
     <definedName name="Адреса_банк_получателя">Export_Contract!$A$34</definedName>
     <definedName name="Адреса_банк_получателя_адрес">Export_Contract!$A$35</definedName>
     <definedName name="Адреса_банк_получателя_свифт">Export_Contract!$A$36</definedName>
@@ -635,9 +635,6 @@
     <t>Изготовитель</t>
   </si>
   <si>
-    <t>Страна происхождения РОССИЯ</t>
-  </si>
-  <si>
     <t>*  МФТ "Морской Волк"
     MSC Икра минтая - 222,021 тн (нетто)</t>
   </si>
@@ -691,6 +688,9 @@
     MSC Молоки минтая мороженые - 29,585 тн (нетто)
 *  МФТ "Морской Волк"
     MSC Икра минтая - 222,021 тн (нетто)</t>
+  </si>
+  <si>
+    <t>СТРАНА ПРОИСХОЖДЕНИЯ РОССИЯ</t>
   </si>
 </sst>
 </file>
@@ -973,7 +973,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1275,6 +1275,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1320,17 +1332,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1650,10 +1653,10 @@
     <tabColor theme="9" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W90"/>
+  <dimension ref="A1:W85"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="140" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A19" zoomScale="140" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1748,11 +1751,11 @@
       <c r="U3" s="9"/>
       <c r="V3" s="9"/>
     </row>
-    <row r="4" spans="1:22" s="124" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="125" t="s">
+    <row r="4" spans="1:22" s="109" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="110" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="126" t="s">
+      <c r="B4" s="111" t="s">
         <v>92</v>
       </c>
       <c r="F4" s="11"/>
@@ -1942,10 +1945,10 @@
     </row>
     <row r="17" spans="1:22" ht="36.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F17"/>
       <c r="G17"/>
@@ -2038,10 +2041,10 @@
     </row>
     <row r="21" spans="1:22" ht="49.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="B21" s="27" t="s">
         <v>160</v>
-      </c>
-      <c r="B21" s="27" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:22" s="12" customFormat="1" ht="54.85" customHeight="1" x14ac:dyDescent="0.45">
@@ -2119,11 +2122,11 @@
       <c r="V26" s="35"/>
     </row>
     <row r="27" spans="1:22" ht="124.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="128" t="s">
+        <v>169</v>
+      </c>
+      <c r="B27" s="128" t="s">
         <v>170</v>
-      </c>
-      <c r="B27" s="19" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.45">
@@ -2295,48 +2298,48 @@
       </c>
     </row>
     <row r="49" spans="1:2" ht="10.9" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="127"/>
-      <c r="B49" s="127"/>
+      <c r="A49" s="112"/>
+      <c r="B49" s="112"/>
     </row>
     <row r="50" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="127"/>
-      <c r="B50" s="127"/>
+      <c r="A50" s="112"/>
+      <c r="B50" s="112"/>
     </row>
     <row r="51" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="127"/>
-      <c r="B51" s="127"/>
+      <c r="A51" s="112"/>
+      <c r="B51" s="112"/>
     </row>
     <row r="52" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="127"/>
-      <c r="B52" s="127"/>
+      <c r="A52" s="112"/>
+      <c r="B52" s="112"/>
     </row>
     <row r="53" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="127"/>
-      <c r="B53" s="127"/>
+      <c r="A53" s="112"/>
+      <c r="B53" s="112"/>
     </row>
     <row r="54" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="127"/>
-      <c r="B54" s="127"/>
+      <c r="A54" s="112"/>
+      <c r="B54" s="112"/>
     </row>
     <row r="55" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="127"/>
-      <c r="B55" s="127"/>
+      <c r="A55" s="112"/>
+      <c r="B55" s="112"/>
     </row>
     <row r="56" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="127"/>
-      <c r="B56" s="127"/>
+      <c r="A56" s="112"/>
+      <c r="B56" s="112"/>
     </row>
     <row r="57" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="127"/>
-      <c r="B57" s="127"/>
+      <c r="A57" s="112"/>
+      <c r="B57" s="112"/>
     </row>
     <row r="58" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="127"/>
-      <c r="B58" s="127"/>
+      <c r="A58" s="112"/>
+      <c r="B58" s="112"/>
     </row>
     <row r="59" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="127"/>
-      <c r="B59" s="127"/>
+      <c r="A59" s="112"/>
+      <c r="B59" s="112"/>
     </row>
     <row r="60" spans="1:2" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="61" spans="1:2" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2344,14 +2347,14 @@
     <row r="63" spans="1:2" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="64" spans="1:2" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="65" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="66" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="67" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="68" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="69" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="70" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="66" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="67" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="68" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="69" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="70" hidden="1" x14ac:dyDescent="0.45"/>
     <row r="71" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="83" ht="26.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="90" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="78" ht="26.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="85" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{13E4E285-FA5D-41CC-AC7F-578EA8AF8279}">
@@ -2364,9 +2367,6 @@
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.11811023622047245" top="0.15748031496062992" bottom="0.15748031496062992" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="91" fitToHeight="0" orientation="portrait" r:id="rId1"/>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="22" max="16383" man="1"/>
-  </rowBreaks>
 </worksheet>
 </file>
 
@@ -2378,8 +2378,8 @@
   </sheetPr>
   <dimension ref="A2:AA112"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A83" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81:H81"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A80" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="E108" sqref="E108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2414,12 +2414,12 @@
       <c r="H2" s="38"/>
     </row>
     <row r="3" spans="1:27" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="117" t="s">
+      <c r="A3" s="121" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="118"/>
-      <c r="C3" s="118"/>
-      <c r="D3" s="118"/>
+      <c r="B3" s="122"/>
+      <c r="C3" s="122"/>
+      <c r="D3" s="122"/>
       <c r="E3" s="39" t="s">
         <v>2</v>
       </c>
@@ -2462,8 +2462,8 @@
       <c r="B5" s="44"/>
       <c r="C5" s="46"/>
       <c r="D5" s="46"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="116"/>
+      <c r="E5" s="119"/>
+      <c r="F5" s="120"/>
       <c r="G5" s="51"/>
       <c r="H5" s="52"/>
       <c r="R5">
@@ -2502,18 +2502,18 @@
       <c r="H7" s="60"/>
     </row>
     <row r="8" spans="1:27" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="109" t="s">
-        <v>168</v>
-      </c>
-      <c r="B8" s="110"/>
-      <c r="C8" s="110"/>
-      <c r="D8" s="111"/>
-      <c r="E8" s="112" t="s">
+      <c r="A8" s="113" t="s">
+        <v>167</v>
+      </c>
+      <c r="B8" s="114"/>
+      <c r="C8" s="114"/>
+      <c r="D8" s="115"/>
+      <c r="E8" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="113"/>
-      <c r="G8" s="113"/>
-      <c r="H8" s="114"/>
+      <c r="F8" s="117"/>
+      <c r="G8" s="117"/>
+      <c r="H8" s="118"/>
     </row>
     <row r="9" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="61" t="s">
@@ -2591,12 +2591,12 @@
     <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="51"/>
       <c r="D14" s="66"/>
-      <c r="E14" s="121" t="s">
+      <c r="E14" s="125" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="122"/>
-      <c r="G14" s="122"/>
-      <c r="H14" s="123"/>
+      <c r="F14" s="126"/>
+      <c r="G14" s="126"/>
+      <c r="H14" s="127"/>
     </row>
     <row r="15" spans="1:27" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="100" t="s">
@@ -2963,25 +2963,25 @@
         <v>48</v>
       </c>
       <c r="D42" s="80" t="s">
+        <v>161</v>
+      </c>
+      <c r="E42" s="81" t="s">
         <v>162</v>
-      </c>
-      <c r="E42" s="81" t="s">
-        <v>163</v>
       </c>
       <c r="G42" s="82"/>
       <c r="H42" s="83" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A43" s="119" t="s">
+      <c r="A43" s="123" t="s">
         <v>49</v>
       </c>
-      <c r="B43" s="120"/>
-      <c r="C43" s="120"/>
-      <c r="D43" s="120"/>
-      <c r="E43" s="120"/>
-      <c r="F43" s="120"/>
+      <c r="B43" s="124"/>
+      <c r="C43" s="124"/>
+      <c r="D43" s="124"/>
+      <c r="E43" s="124"/>
+      <c r="F43" s="124"/>
       <c r="G43" s="82"/>
       <c r="H43" s="66"/>
     </row>
@@ -3238,18 +3238,18 @@
       <c r="H72" s="60"/>
     </row>
     <row r="73" spans="1:8" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A73" s="112" t="s">
+      <c r="A73" s="116" t="s">
         <v>15</v>
       </c>
-      <c r="B73" s="113"/>
-      <c r="C73" s="113"/>
-      <c r="D73" s="114"/>
-      <c r="E73" s="112" t="s">
+      <c r="B73" s="117"/>
+      <c r="C73" s="117"/>
+      <c r="D73" s="118"/>
+      <c r="E73" s="116" t="s">
         <v>146</v>
       </c>
-      <c r="F73" s="113"/>
-      <c r="G73" s="113"/>
-      <c r="H73" s="114"/>
+      <c r="F73" s="117"/>
+      <c r="G73" s="117"/>
+      <c r="H73" s="118"/>
     </row>
     <row r="74" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="95" t="s">
@@ -3601,8 +3601,8 @@
       <c r="H103" s="7"/>
     </row>
     <row r="104" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A104" s="5" t="s">
-        <v>158</v>
+      <c r="A104" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="B104" s="6"/>
       <c r="C104" s="6"/>
@@ -3631,25 +3631,25 @@
         <v>87</v>
       </c>
       <c r="D106" s="80" t="s">
+        <v>164</v>
+      </c>
+      <c r="E106" s="105" t="s">
         <v>165</v>
-      </c>
-      <c r="E106" s="105" t="s">
-        <v>166</v>
       </c>
       <c r="G106" s="82"/>
       <c r="H106" s="83" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A107" s="119" t="s">
+      <c r="A107" s="123" t="s">
         <v>49</v>
       </c>
-      <c r="B107" s="120"/>
-      <c r="C107" s="120"/>
-      <c r="D107" s="120"/>
-      <c r="E107" s="120"/>
-      <c r="F107" s="120"/>
+      <c r="B107" s="124"/>
+      <c r="C107" s="124"/>
+      <c r="D107" s="124"/>
+      <c r="E107" s="124"/>
+      <c r="F107" s="124"/>
       <c r="G107" s="82"/>
       <c r="H107" s="66"/>
     </row>

</xml_diff>

<commit_message>
templates export contract minor bugs fixed
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement_Vessels.xlsx
+++ b/templates/Export_Agreement_Vessels.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527C55F5-0C92-4D65-8A48-A46CF3D7A268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B889CF1-144A-4077-BB63-9CC4879C3552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-55778" yWindow="-907" windowWidth="28995" windowHeight="15795" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="-52882" yWindow="3045" windowWidth="13425" windowHeight="7800" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
     <sheet name="Com_Invoice" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Com_Invoice!$A$1:$J$129</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Export_Contract!$A$1:$B$65</definedName>
     <definedName name="Адреса_банк_получателя">Export_Contract!$A$34</definedName>
     <definedName name="Адреса_банк_получателя_адрес">Export_Contract!$A$35</definedName>
@@ -40,78 +41,78 @@
     <definedName name="Доставка_заголовок">Export_Contract!$A$23</definedName>
     <definedName name="Доставка_порт">Export_Contract!$A$25</definedName>
     <definedName name="Доставка_условия">Export_Contract!$A$24</definedName>
-    <definedName name="Инвойс">Com_Invoice!$E$4</definedName>
-    <definedName name="Инвойс_Bl_массив">Com_Invoice!$A$16</definedName>
-    <definedName name="Инвойс_Bl_массив_п">Com_Invoice!$A$81</definedName>
-    <definedName name="Инвойс_банк_получателя">Com_Invoice!$A$44</definedName>
-    <definedName name="Инвойс_банк_получателя_адрес">Com_Invoice!$A$45</definedName>
-    <definedName name="Инвойс_банк_получателя_адрес_п">Com_Invoice!$A$109</definedName>
-    <definedName name="Инвойс_банк_получателя_п">Com_Invoice!$A$108</definedName>
-    <definedName name="Инвойс_банк_получателя_свифт">Com_Invoice!$A$46</definedName>
-    <definedName name="Инвойс_банк_получателя_свифт_п">Com_Invoice!$A$110</definedName>
-    <definedName name="Инвойс_всего">Com_Invoice!$F$16</definedName>
-    <definedName name="Инвойс_всего_п">Com_Invoice!$F$81</definedName>
-    <definedName name="Инвойс_дата">Com_Invoice!$A$10</definedName>
-    <definedName name="Инвойс_дата_п">Com_Invoice!$A$75</definedName>
-    <definedName name="Инвойс_декларация">Com_Invoice!$A$13</definedName>
-    <definedName name="Инвойс_декларация_п">Com_Invoice!$A$78</definedName>
-    <definedName name="Инвойс_контракт">Com_Invoice!$E$11</definedName>
-    <definedName name="Инвойс_контракт_дата">Com_Invoice!$E$12</definedName>
-    <definedName name="Инвойс_контракт_дата_п">Com_Invoice!$E$77</definedName>
-    <definedName name="Инвойс_контракт_п">Com_Invoice!$E$76</definedName>
-    <definedName name="Инвойс_куда">Com_Invoice!$A$12</definedName>
-    <definedName name="Инвойс_куда_п">Com_Invoice!$A$77</definedName>
-    <definedName name="Инвойс_места">Com_Invoice!$E$16</definedName>
-    <definedName name="Инвойс_места_п">Com_Invoice!$E$81</definedName>
-    <definedName name="Инвойс_откуда">Com_Invoice!$B$12</definedName>
-    <definedName name="Инвойс_откуда_п">Com_Invoice!$B$77</definedName>
-    <definedName name="Инвойс_п">Com_Invoice!$E$69</definedName>
-    <definedName name="Инвойс_подвал_всего">Com_Invoice!$E$42</definedName>
-    <definedName name="Инвойс_подвал_всего_п">Com_Invoice!$E$106</definedName>
-    <definedName name="Инвойс_подвал_места">Com_Invoice!$D$42</definedName>
-    <definedName name="Инвойс_подвал_места_п">Com_Invoice!$D$106</definedName>
-    <definedName name="Инвойс_подвал_сумма">Com_Invoice!$H$42</definedName>
-    <definedName name="Инвойс_подвал_сумма_п">Com_Invoice!$H$106</definedName>
-    <definedName name="Инвойс_подписант">Com_Invoice!$E$44</definedName>
-    <definedName name="Инвойс_подписант_п">Com_Invoice!$E$108</definedName>
-    <definedName name="Инвойс_покупатель">Com_Invoice!$E$7</definedName>
-    <definedName name="Инвойс_покупатель_адрес">Com_Invoice!$E$8</definedName>
-    <definedName name="Инвойс_покупатель_адрес_п">Com_Invoice!$E$73</definedName>
-    <definedName name="Инвойс_покупатель_п">Com_Invoice!$E$72</definedName>
-    <definedName name="Инвойс_получатель">Com_Invoice!$A$7</definedName>
-    <definedName name="Инвойс_получатель_адрес">Com_Invoice!$A$8</definedName>
-    <definedName name="Инвойс_получатель_адрес_п">Com_Invoice!$A$73</definedName>
-    <definedName name="Инвойс_получатель_в_пользу">Com_Invoice!$A$47</definedName>
-    <definedName name="Инвойс_получатель_в_пользу_п">Com_Invoice!$A$111</definedName>
-    <definedName name="Инвойс_получатель_п">Com_Invoice!$A$72</definedName>
-    <definedName name="Инвойс_получатель_счет">Com_Invoice!$A$48</definedName>
-    <definedName name="Инвойс_получатель_счет_п">Com_Invoice!$A$112</definedName>
-    <definedName name="Инвойс_продавец">Com_Invoice!$A$4</definedName>
-    <definedName name="Инвойс_продавец_адрес">Com_Invoice!$A$5</definedName>
-    <definedName name="Инвойс_продавец_адрес_п">Com_Invoice!$A$70</definedName>
-    <definedName name="Инвойс_продавец_п">Com_Invoice!$A$69</definedName>
-    <definedName name="Инвойс_продукт">Com_Invoice!$C$16</definedName>
-    <definedName name="Инвойс_продукт_п">Com_Invoice!$C$81</definedName>
-    <definedName name="Инвойс_соглашение">Com_Invoice!$E$10</definedName>
-    <definedName name="Инвойс_соглашение_п">Com_Invoice!$E$75</definedName>
-    <definedName name="Инвойс_судно">Com_Invoice!$A$39</definedName>
-    <definedName name="Инвойс_судно_п">Com_Invoice!$A$103</definedName>
-    <definedName name="Инвойс_сумма">Com_Invoice!$H$16</definedName>
-    <definedName name="Инвойс_сумма_п">Com_Invoice!$H$81</definedName>
-    <definedName name="Инвойс_транспорт">Com_Invoice!$B$10</definedName>
-    <definedName name="Инвойс_транспорт_п">Com_Invoice!$B$75</definedName>
-    <definedName name="Инвойс_упаковка">Com_Invoice!$D$16</definedName>
-    <definedName name="Инвойс_упаковка_п">Com_Invoice!$D$81</definedName>
-    <definedName name="Инвойс_условия">Com_Invoice!$E$14</definedName>
-    <definedName name="Инвойс_условия_п">Com_Invoice!$E$79</definedName>
-    <definedName name="Инвойс_цена">Com_Invoice!$G$16</definedName>
-    <definedName name="Инвойс_цена_п">Com_Invoice!$G$81</definedName>
+    <definedName name="Инвойс">Com_Invoice!$F$4</definedName>
+    <definedName name="Инвойс_Bl_массив">Com_Invoice!$B$16</definedName>
+    <definedName name="Инвойс_Bl_массив_п">Com_Invoice!$B$85</definedName>
+    <definedName name="Инвойс_банк_получателя">Com_Invoice!$B$44</definedName>
+    <definedName name="Инвойс_банк_получателя_адрес">Com_Invoice!$B$45</definedName>
+    <definedName name="Инвойс_банк_получателя_адрес_п">Com_Invoice!$B$113</definedName>
+    <definedName name="Инвойс_банк_получателя_п">Com_Invoice!$B$112</definedName>
+    <definedName name="Инвойс_банк_получателя_свифт">Com_Invoice!$B$46</definedName>
+    <definedName name="Инвойс_банк_получателя_свифт_п">Com_Invoice!$B$114</definedName>
+    <definedName name="Инвойс_всего">Com_Invoice!$G$16</definedName>
+    <definedName name="Инвойс_всего_п">Com_Invoice!$G$85</definedName>
+    <definedName name="Инвойс_дата">Com_Invoice!$B$10</definedName>
+    <definedName name="Инвойс_дата_п">Com_Invoice!$B$79</definedName>
+    <definedName name="Инвойс_декларация">Com_Invoice!$B$13</definedName>
+    <definedName name="Инвойс_декларация_п">Com_Invoice!$B$82</definedName>
+    <definedName name="Инвойс_контракт">Com_Invoice!$F$11</definedName>
+    <definedName name="Инвойс_контракт_дата">Com_Invoice!$F$12</definedName>
+    <definedName name="Инвойс_контракт_дата_п">Com_Invoice!$F$81</definedName>
+    <definedName name="Инвойс_контракт_п">Com_Invoice!$F$80</definedName>
+    <definedName name="Инвойс_куда">Com_Invoice!$B$12</definedName>
+    <definedName name="Инвойс_куда_п">Com_Invoice!$B$81</definedName>
+    <definedName name="Инвойс_места">Com_Invoice!$F$16</definedName>
+    <definedName name="Инвойс_места_п">Com_Invoice!$F$85</definedName>
+    <definedName name="Инвойс_откуда">Com_Invoice!$C$12</definedName>
+    <definedName name="Инвойс_откуда_п">Com_Invoice!$C$81</definedName>
+    <definedName name="Инвойс_п">Com_Invoice!$F$73</definedName>
+    <definedName name="Инвойс_подвал_всего">Com_Invoice!$F$42</definedName>
+    <definedName name="Инвойс_подвал_всего_п">Com_Invoice!$F$110</definedName>
+    <definedName name="Инвойс_подвал_места">Com_Invoice!$E$42</definedName>
+    <definedName name="Инвойс_подвал_места_п">Com_Invoice!$E$110</definedName>
+    <definedName name="Инвойс_подвал_сумма">Com_Invoice!$I$42</definedName>
+    <definedName name="Инвойс_подвал_сумма_п">Com_Invoice!$I$110</definedName>
+    <definedName name="Инвойс_подписант">Com_Invoice!$F$44</definedName>
+    <definedName name="Инвойс_подписант_п">Com_Invoice!$F$112</definedName>
+    <definedName name="Инвойс_покупатель">Com_Invoice!$F$7</definedName>
+    <definedName name="Инвойс_покупатель_адрес">Com_Invoice!$F$8</definedName>
+    <definedName name="Инвойс_покупатель_адрес_п">Com_Invoice!$F$77</definedName>
+    <definedName name="Инвойс_покупатель_п">Com_Invoice!$F$76</definedName>
+    <definedName name="Инвойс_получатель">Com_Invoice!$B$7</definedName>
+    <definedName name="Инвойс_получатель_адрес">Com_Invoice!$B$8</definedName>
+    <definedName name="Инвойс_получатель_адрес_п">Com_Invoice!$B$77</definedName>
+    <definedName name="Инвойс_получатель_в_пользу">Com_Invoice!$B$47</definedName>
+    <definedName name="Инвойс_получатель_в_пользу_п">Com_Invoice!$B$115</definedName>
+    <definedName name="Инвойс_получатель_п">Com_Invoice!$B$76</definedName>
+    <definedName name="Инвойс_получатель_счет">Com_Invoice!$B$48</definedName>
+    <definedName name="Инвойс_получатель_счет_п">Com_Invoice!$B$116</definedName>
+    <definedName name="Инвойс_продавец">Com_Invoice!$B$4</definedName>
+    <definedName name="Инвойс_продавец_адрес">Com_Invoice!$B$5</definedName>
+    <definedName name="Инвойс_продавец_адрес_п">Com_Invoice!$B$74</definedName>
+    <definedName name="Инвойс_продавец_п">Com_Invoice!$B$73</definedName>
+    <definedName name="Инвойс_продукт">Com_Invoice!$D$16</definedName>
+    <definedName name="Инвойс_продукт_п">Com_Invoice!$D$85</definedName>
+    <definedName name="Инвойс_соглашение">Com_Invoice!$F$10</definedName>
+    <definedName name="Инвойс_соглашение_п">Com_Invoice!$F$79</definedName>
+    <definedName name="Инвойс_судно">Com_Invoice!$B$39</definedName>
+    <definedName name="Инвойс_судно_п">Com_Invoice!$B$107</definedName>
+    <definedName name="Инвойс_сумма">Com_Invoice!$I$16</definedName>
+    <definedName name="Инвойс_сумма_п">Com_Invoice!$I$85</definedName>
+    <definedName name="Инвойс_транспорт">Com_Invoice!$C$10</definedName>
+    <definedName name="Инвойс_транспорт_п">Com_Invoice!$C$79</definedName>
+    <definedName name="Инвойс_упаковка">Com_Invoice!$E$16</definedName>
+    <definedName name="Инвойс_упаковка_п">Com_Invoice!$E$85</definedName>
+    <definedName name="Инвойс_условия">Com_Invoice!$F$14</definedName>
+    <definedName name="Инвойс_условия_п">Com_Invoice!$F$83</definedName>
+    <definedName name="Инвойс_цена">Com_Invoice!$H$16</definedName>
+    <definedName name="Инвойс_цена_п">Com_Invoice!$H$85</definedName>
     <definedName name="Контракт">Export_Contract!$A$2</definedName>
     <definedName name="Контракт_дата">Export_Contract!$A$3</definedName>
-    <definedName name="МСЦ">Com_Invoice!$G$4</definedName>
-    <definedName name="МСЦ_п">Com_Invoice!$G$69</definedName>
-    <definedName name="МСЦ_сертификат">Com_Invoice!$H$4</definedName>
-    <definedName name="МСЦ_сертификат_п">Com_Invoice!$H$69</definedName>
+    <definedName name="МСЦ">Com_Invoice!$H$4</definedName>
+    <definedName name="МСЦ_п">Com_Invoice!$H$73</definedName>
+    <definedName name="МСЦ_сертификат">Com_Invoice!$I$4</definedName>
+    <definedName name="МСЦ_сертификат_п">Com_Invoice!$I$73</definedName>
     <definedName name="Покупатель">Export_Contract!$A$11</definedName>
     <definedName name="Покупатель_адрес">Export_Contract!$A$12</definedName>
     <definedName name="Покупатель_заголовок">Export_Contract!$A$10</definedName>
@@ -973,7 +974,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -986,9 +987,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="top"/>
@@ -1233,14 +1231,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1287,6 +1279,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1332,8 +1327,39 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1655,40 +1681,40 @@
   </sheetPr>
   <dimension ref="A1:W85"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A19" zoomScale="140" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A22" zoomScale="140" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="54.6640625" style="31" customWidth="1"/>
+    <col min="1" max="2" width="54.6640625" style="30" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="9" style="8" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" style="8" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="20.33203125" style="8" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" style="8" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="15.796875" style="8" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="49.796875" style="8" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" style="8" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="13.796875" style="8" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="7.33203125" style="8" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="9.796875" style="8" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="23.33203125" style="8" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="0" style="8" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="17.6640625" style="8" customWidth="1"/>
-    <col min="20" max="20" width="13.1328125" style="8" customWidth="1"/>
-    <col min="21" max="21" width="9.06640625" style="8" customWidth="1"/>
-    <col min="22" max="22" width="35.3984375" style="8" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="9" style="7" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" style="7" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" style="7" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" style="7" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="15.796875" style="7" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="49.796875" style="7" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" style="7" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="13.796875" style="7" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="7.33203125" style="7" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="9.796875" style="7" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="23.33203125" style="7" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="0" style="7" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="17.6640625" style="7" customWidth="1"/>
+    <col min="20" max="20" width="13.1328125" style="7" customWidth="1"/>
+    <col min="21" max="21" width="9.06640625" style="7" customWidth="1"/>
+    <col min="22" max="22" width="35.3984375" style="7" customWidth="1"/>
     <col min="23" max="23" width="9.1328125" hidden="1" customWidth="1"/>
     <col min="24" max="24" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>149</v>
       </c>
       <c r="D1" s="1"/>
@@ -1706,10 +1732,10 @@
       <c r="R1"/>
     </row>
     <row r="2" spans="1:22" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>89</v>
       </c>
       <c r="D2" s="1"/>
@@ -1727,48 +1753,48 @@
       <c r="R2"/>
     </row>
     <row r="3" spans="1:22" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
-    </row>
-    <row r="4" spans="1:22" s="109" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="110" t="s">
+      <c r="F3" s="8"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+    </row>
+    <row r="4" spans="1:22" s="106" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="107" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="111" t="s">
+      <c r="B4" s="108" t="s">
         <v>92</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
+      <c r="F4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
     </row>
     <row r="5" spans="1:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>94</v>
       </c>
       <c r="D5" s="1"/>
@@ -1786,10 +1812,10 @@
       <c r="R5"/>
     </row>
     <row r="6" spans="1:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22" t="s">
         <v>59</v>
       </c>
       <c r="G6"/>
@@ -1806,29 +1832,29 @@
       <c r="R6"/>
     </row>
     <row r="7" spans="1:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="18" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="18" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="F9" s="11"/>
+      <c r="F9" s="10"/>
       <c r="G9"/>
       <c r="H9"/>
       <c r="I9"/>
@@ -1841,16 +1867,16 @@
       <c r="P9"/>
       <c r="Q9"/>
       <c r="R9"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
     </row>
     <row r="10" spans="1:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="20" t="s">
         <v>98</v>
       </c>
       <c r="G10"/>
@@ -1867,10 +1893,10 @@
       <c r="R10"/>
     </row>
     <row r="11" spans="1:22" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="22" t="s">
         <v>12</v>
       </c>
       <c r="G11"/>
@@ -1887,42 +1913,42 @@
       <c r="R11"/>
     </row>
     <row r="12" spans="1:22" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="18" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="18" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="24" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="18" t="s">
         <v>151</v>
       </c>
       <c r="F16"/>
@@ -1944,10 +1970,10 @@
       <c r="V16"/>
     </row>
     <row r="17" spans="1:22" ht="36.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="18" t="s">
         <v>158</v>
       </c>
       <c r="F17"/>
@@ -1969,8 +1995,8 @@
       <c r="V17"/>
     </row>
     <row r="18" spans="1:22" ht="10.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="18"/>
-      <c r="B18" s="19"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="18"/>
       <c r="F18"/>
       <c r="G18"/>
       <c r="H18"/>
@@ -1990,10 +2016,10 @@
       <c r="V18"/>
     </row>
     <row r="19" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="24" t="s">
         <v>106</v>
       </c>
       <c r="F19"/>
@@ -2015,10 +2041,10 @@
       <c r="V19"/>
     </row>
     <row r="20" spans="1:22" ht="25.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="18" t="s">
         <v>108</v>
       </c>
       <c r="F20"/>
@@ -2040,306 +2066,306 @@
       <c r="V20"/>
     </row>
     <row r="21" spans="1:22" ht="49.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="26" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="22" spans="1:22" s="12" customFormat="1" ht="54.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="36" t="s">
+    <row r="22" spans="1:22" s="11" customFormat="1" ht="54.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="13"/>
-      <c r="S22" s="13"/>
-      <c r="T22" s="13"/>
-      <c r="U22" s="13"/>
-      <c r="V22" s="13"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="12"/>
+      <c r="T22" s="12"/>
+      <c r="U22" s="12"/>
+      <c r="V22" s="12"/>
     </row>
     <row r="23" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="31" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:22" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="18" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:22" ht="38.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="18" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:22" s="34" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="33" t="s">
+    <row r="26" spans="1:22" s="33" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="B26" s="33" t="s">
+      <c r="B26" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="35"/>
-      <c r="J26" s="35"/>
-      <c r="K26" s="35"/>
-      <c r="L26" s="35"/>
-      <c r="M26" s="35"/>
-      <c r="N26" s="35"/>
-      <c r="O26" s="35"/>
-      <c r="P26" s="35"/>
-      <c r="Q26" s="35"/>
-      <c r="R26" s="35"/>
-      <c r="S26" s="35"/>
-      <c r="T26" s="35"/>
-      <c r="U26" s="35"/>
-      <c r="V26" s="35"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="34"/>
+      <c r="L26" s="34"/>
+      <c r="M26" s="34"/>
+      <c r="N26" s="34"/>
+      <c r="O26" s="34"/>
+      <c r="P26" s="34"/>
+      <c r="Q26" s="34"/>
+      <c r="R26" s="34"/>
+      <c r="S26" s="34"/>
+      <c r="T26" s="34"/>
+      <c r="U26" s="34"/>
+      <c r="V26" s="34"/>
     </row>
     <row r="27" spans="1:22" ht="124.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="128" t="s">
+      <c r="A27" s="110" t="s">
         <v>169</v>
       </c>
-      <c r="B27" s="128" t="s">
+      <c r="B27" s="110" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="24" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="18" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="24" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="22" t="s">
+      <c r="A31" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="B31" s="23" t="s">
+      <c r="B31" s="22" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:22" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="22" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="18" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="18" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="18" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="18" t="s">
+      <c r="A37" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B37" s="19" t="s">
+      <c r="B37" s="18" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="18" t="s">
+      <c r="A38" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="B38" s="19" t="s">
+      <c r="B38" s="18" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="22" t="s">
+      <c r="A39" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="B39" s="23" t="s">
+      <c r="B39" s="22" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="22" t="s">
+      <c r="A40" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="23" t="s">
+      <c r="B40" s="22" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="25.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="18" t="s">
+      <c r="A41" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="18" t="s">
+      <c r="A42" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="18" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="18" t="s">
+      <c r="A43" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="B43" s="19" t="s">
+      <c r="B43" s="18" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="18" t="s">
+      <c r="A44" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="B44" s="19" t="s">
+      <c r="B44" s="18" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="18" t="s">
+      <c r="A45" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="B45" s="19" t="s">
+      <c r="B45" s="18" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="18" t="s">
+      <c r="A46" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="B46" s="19" t="s">
+      <c r="B46" s="18" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="28" t="s">
+      <c r="A47" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="B47" s="29" t="s">
+      <c r="B47" s="28" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="30" t="s">
+      <c r="A48" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="B48" s="30" t="s">
+      <c r="B48" s="29" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="10.9" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="112"/>
-      <c r="B49" s="112"/>
+      <c r="A49" s="109"/>
+      <c r="B49" s="109"/>
     </row>
     <row r="50" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="112"/>
-      <c r="B50" s="112"/>
+      <c r="A50" s="109"/>
+      <c r="B50" s="109"/>
     </row>
     <row r="51" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="112"/>
-      <c r="B51" s="112"/>
+      <c r="A51" s="109"/>
+      <c r="B51" s="109"/>
     </row>
     <row r="52" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="112"/>
-      <c r="B52" s="112"/>
+      <c r="A52" s="109"/>
+      <c r="B52" s="109"/>
     </row>
     <row r="53" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="112"/>
-      <c r="B53" s="112"/>
+      <c r="A53" s="109"/>
+      <c r="B53" s="109"/>
     </row>
     <row r="54" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="112"/>
-      <c r="B54" s="112"/>
+      <c r="A54" s="109"/>
+      <c r="B54" s="109"/>
     </row>
     <row r="55" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="112"/>
-      <c r="B55" s="112"/>
+      <c r="A55" s="109"/>
+      <c r="B55" s="109"/>
     </row>
     <row r="56" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="112"/>
-      <c r="B56" s="112"/>
+      <c r="A56" s="109"/>
+      <c r="B56" s="109"/>
     </row>
     <row r="57" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="112"/>
-      <c r="B57" s="112"/>
+      <c r="A57" s="109"/>
+      <c r="B57" s="109"/>
     </row>
     <row r="58" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="112"/>
-      <c r="B58" s="112"/>
+      <c r="A58" s="109"/>
+      <c r="B58" s="109"/>
     </row>
     <row r="59" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="112"/>
-      <c r="B59" s="112"/>
+      <c r="A59" s="109"/>
+      <c r="B59" s="109"/>
     </row>
     <row r="60" spans="1:2" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="61" spans="1:2" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2376,1353 +2402,1574 @@
     <tabColor theme="9" tint="-0.499984740745262"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:AA112"/>
+  <dimension ref="A2:AB129"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A80" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="E108" sqref="E108"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A42" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.06640625" customWidth="1"/>
-    <col min="2" max="2" width="20.1328125" customWidth="1"/>
-    <col min="3" max="3" width="26.06640625" customWidth="1"/>
-    <col min="4" max="4" width="11.06640625" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
-    <col min="8" max="8" width="18.796875" customWidth="1"/>
-    <col min="18" max="18" width="0" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="25.6640625" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="23.33203125" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="25.33203125" hidden="1" customWidth="1"/>
-    <col min="22" max="23" width="0" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="10.33203125" hidden="1" customWidth="1"/>
-    <col min="25" max="28" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="2.53125" customWidth="1"/>
+    <col min="2" max="2" width="14.06640625" customWidth="1"/>
+    <col min="3" max="3" width="20.1328125" customWidth="1"/>
+    <col min="4" max="4" width="26.06640625" customWidth="1"/>
+    <col min="5" max="5" width="11.06640625" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="9" max="9" width="18.796875" customWidth="1"/>
+    <col min="10" max="10" width="2.3984375" customWidth="1"/>
+    <col min="19" max="19" width="0" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="25.6640625" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="23.33203125" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="25.33203125" hidden="1" customWidth="1"/>
+    <col min="23" max="24" width="0" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="10.33203125" hidden="1" customWidth="1"/>
+    <col min="26" max="29" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:27" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="106" t="s">
+    <row r="2" spans="1:28" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-    </row>
-    <row r="3" spans="1:27" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="121" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+    </row>
+    <row r="3" spans="1:28" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="51"/>
+      <c r="B3" s="119" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="122"/>
-      <c r="C3" s="122"/>
-      <c r="D3" s="122"/>
-      <c r="E3" s="39" t="s">
+      <c r="C3" s="120"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="40"/>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="39"/>
+      <c r="H3" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="42" t="s">
+      <c r="I3" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="R3">
+      <c r="J3" s="50"/>
+      <c r="S3">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="43" t="s">
+    <row r="4" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="51"/>
+      <c r="B4" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="47" t="s">
+      <c r="C4" s="43"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="48"/>
-      <c r="G4" s="49" t="s">
+      <c r="G4" s="47"/>
+      <c r="H4" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="50" t="s">
+      <c r="I4" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="R4">
+      <c r="J4" s="50"/>
+      <c r="S4">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="43" t="s">
+    <row r="5" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="51"/>
+      <c r="B5" s="42" t="s">
         <v>152</v>
       </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="119"/>
-      <c r="F5" s="120"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="52"/>
-      <c r="R5">
+      <c r="C5" s="43"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="117"/>
+      <c r="G5" s="118"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="50"/>
+      <c r="S5">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="53" t="s">
+    <row r="6" spans="1:28" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="51"/>
+      <c r="B6" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="53" t="s">
+      <c r="C6" s="53"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="56"/>
-      <c r="R6">
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="50"/>
+      <c r="S6">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="47" t="s">
+    <row r="7" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="51"/>
+      <c r="B7" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="48"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="59" t="s">
+      <c r="C7" s="47"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="60"/>
-    </row>
-    <row r="8" spans="1:27" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="113" t="s">
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="50"/>
+    </row>
+    <row r="8" spans="1:28" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="51"/>
+      <c r="B8" s="111" t="s">
         <v>167</v>
       </c>
-      <c r="B8" s="114"/>
-      <c r="C8" s="114"/>
-      <c r="D8" s="115"/>
-      <c r="E8" s="116" t="s">
+      <c r="C8" s="112"/>
+      <c r="D8" s="112"/>
+      <c r="E8" s="113"/>
+      <c r="F8" s="114" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="117"/>
-      <c r="G8" s="117"/>
-      <c r="H8" s="118"/>
-    </row>
-    <row r="9" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="61" t="s">
+      <c r="G8" s="115"/>
+      <c r="H8" s="115"/>
+      <c r="I8" s="116"/>
+      <c r="J8" s="50"/>
+    </row>
+    <row r="9" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="51"/>
+      <c r="B9" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="C9" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="52"/>
-      <c r="E9" s="53" t="s">
+      <c r="E9" s="51"/>
+      <c r="F9" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="54"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="56"/>
-    </row>
-    <row r="10" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="62" t="s">
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="50"/>
+    </row>
+    <row r="10" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="51"/>
+      <c r="B10" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="63" t="s">
+      <c r="C10" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="52"/>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="51"/>
+      <c r="F10" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="65"/>
-    </row>
-    <row r="11" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="61" t="s">
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="64"/>
+      <c r="J10" s="50"/>
+    </row>
+    <row r="11" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="51"/>
+      <c r="B11" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="C11" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="66"/>
-      <c r="E11" s="59" t="s">
+      <c r="E11" s="65"/>
+      <c r="F11" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="60"/>
-    </row>
-    <row r="12" spans="1:27" ht="34.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="67" t="s">
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="50"/>
+    </row>
+    <row r="12" spans="1:28" ht="34.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="51"/>
+      <c r="B12" s="66" t="s">
         <v>147</v>
       </c>
-      <c r="B12" s="68" t="s">
+      <c r="C12" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="69"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="71" t="s">
+      <c r="D12" s="68"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="72"/>
-      <c r="G12" s="72"/>
-      <c r="H12" s="73"/>
-    </row>
-    <row r="13" spans="1:27" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="51" t="s">
+      <c r="G12" s="71"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="72"/>
+      <c r="J12" s="50"/>
+    </row>
+    <row r="13" spans="1:28" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="51"/>
+      <c r="B13" s="50" t="s">
         <v>153</v>
       </c>
-      <c r="D13" s="66"/>
-      <c r="E13" s="53" t="s">
+      <c r="E13" s="65"/>
+      <c r="F13" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="56"/>
-    </row>
-    <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="50"/>
+    </row>
+    <row r="14" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="51"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="125" t="s">
+      <c r="B14" s="50"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="123" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="126"/>
-      <c r="G14" s="126"/>
-      <c r="H14" s="127"/>
-    </row>
-    <row r="15" spans="1:27" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="100" t="s">
+      <c r="G14" s="124"/>
+      <c r="H14" s="124"/>
+      <c r="I14" s="125"/>
+      <c r="J14" s="50"/>
+    </row>
+    <row r="15" spans="1:28" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="51"/>
+      <c r="B15" s="97" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="101" t="s">
+      <c r="C15" s="98" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="101" t="s">
+      <c r="D15" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="101" t="s">
+      <c r="E15" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="108" t="s">
+      <c r="F15" s="105" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="108"/>
-      <c r="G15" s="101" t="s">
+      <c r="G15" s="105"/>
+      <c r="H15" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="H15" s="103" t="s">
+      <c r="I15" s="100" t="s">
         <v>34</v>
       </c>
-      <c r="R15" t="s">
+      <c r="J15" s="50"/>
+      <c r="S15" t="s">
         <v>35</v>
       </c>
-      <c r="S15" t="s">
+      <c r="T15" t="s">
         <v>36</v>
       </c>
-      <c r="T15" t="s">
+      <c r="U15" t="s">
         <v>37</v>
       </c>
-      <c r="U15" t="s">
+      <c r="V15" t="s">
         <v>38</v>
       </c>
-      <c r="V15">
+      <c r="W15">
         <v>426</v>
       </c>
-      <c r="W15">
+      <c r="X15">
         <v>9.5850000000000009</v>
       </c>
-      <c r="X15">
+      <c r="Y15">
         <v>3500</v>
       </c>
-      <c r="Y15">
+      <c r="Z15">
         <v>33547.5</v>
       </c>
-      <c r="Z15">
+      <c r="AA15">
         <v>0</v>
       </c>
-      <c r="AA15" t="s">
+      <c r="AB15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="42" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="49" t="s">
+    <row r="16" spans="1:28" ht="42" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="51"/>
+      <c r="B16" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="74" t="s">
+      <c r="C16" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="74" t="s">
+      <c r="D16" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="74" t="s">
+      <c r="E16" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="74" t="s">
+      <c r="F16" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="74" t="s">
+      <c r="G16" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="G16" s="74" t="s">
+      <c r="H16" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="H16" s="50" t="s">
+      <c r="I16" s="49" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A17" s="49"/>
-      <c r="B17" s="74"/>
-      <c r="C17" s="74"/>
-      <c r="D17" s="74"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="74"/>
-      <c r="G17" s="74"/>
-      <c r="H17" s="50"/>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A18" s="49"/>
-      <c r="B18" s="74"/>
-      <c r="C18" s="74"/>
-      <c r="D18" s="74"/>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74"/>
-      <c r="H18" s="50"/>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A19" s="49"/>
-      <c r="B19" s="74"/>
-      <c r="C19" s="74"/>
-      <c r="D19" s="74"/>
-      <c r="E19" s="74"/>
-      <c r="F19" s="74"/>
-      <c r="G19" s="74"/>
-      <c r="H19" s="50"/>
-      <c r="R19" t="s">
+      <c r="J16" s="50"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A17" s="51"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="73"/>
+      <c r="H17" s="73"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="50"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A18" s="51"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="73"/>
+      <c r="H18" s="73"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="50"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A19" s="51"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="73"/>
+      <c r="D19" s="73"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="73"/>
+      <c r="H19" s="73"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="50"/>
+      <c r="S19" t="s">
         <v>35</v>
       </c>
-      <c r="S19" t="s">
+      <c r="T19" t="s">
         <v>37</v>
       </c>
-      <c r="T19">
+      <c r="U19">
         <v>22.500000000000004</v>
       </c>
-      <c r="U19">
+      <c r="V19">
         <v>426</v>
       </c>
-      <c r="V19">
+      <c r="W19">
         <v>9.5850000000000009</v>
       </c>
-      <c r="W19">
+      <c r="X19">
         <v>3500</v>
       </c>
-      <c r="X19">
+      <c r="Y19">
         <v>33547.5</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A20" s="49"/>
-      <c r="B20" s="74"/>
-      <c r="C20" s="74"/>
-      <c r="D20" s="74"/>
-      <c r="E20" s="74"/>
-      <c r="F20" s="74"/>
-      <c r="G20" s="74"/>
-      <c r="H20" s="50"/>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A21" s="49"/>
-      <c r="B21" s="74"/>
-      <c r="C21" s="74"/>
-      <c r="D21" s="74"/>
-      <c r="E21" s="74"/>
-      <c r="F21" s="74"/>
-      <c r="G21" s="74"/>
-      <c r="H21" s="50"/>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A22" s="49"/>
-      <c r="B22" s="74"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="74"/>
-      <c r="H22" s="50"/>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A23" s="49"/>
-      <c r="B23" s="74"/>
-      <c r="C23" s="74"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="50"/>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A24" s="49"/>
-      <c r="B24" s="74"/>
-      <c r="C24" s="74"/>
-      <c r="D24" s="74"/>
-      <c r="E24" s="74"/>
-      <c r="F24" s="74"/>
-      <c r="G24" s="74"/>
-      <c r="H24" s="50"/>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A25" s="49"/>
-      <c r="B25" s="74"/>
-      <c r="C25" s="74"/>
-      <c r="D25" s="74"/>
-      <c r="E25" s="74"/>
-      <c r="F25" s="74"/>
-      <c r="G25" s="74"/>
-      <c r="H25" s="50"/>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A26" s="49"/>
-      <c r="B26" s="74"/>
-      <c r="C26" s="74"/>
-      <c r="D26" s="74"/>
-      <c r="E26" s="74"/>
-      <c r="F26" s="74"/>
-      <c r="G26" s="74"/>
-      <c r="H26" s="50"/>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A27" s="49"/>
-      <c r="B27" s="74"/>
-      <c r="C27" s="74"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="74"/>
-      <c r="F27" s="74"/>
-      <c r="G27" s="74"/>
-      <c r="H27" s="50"/>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A28" s="49"/>
-      <c r="B28" s="74"/>
-      <c r="C28" s="74"/>
-      <c r="D28" s="74"/>
-      <c r="E28" s="74"/>
-      <c r="F28" s="74"/>
-      <c r="G28" s="74"/>
-      <c r="H28" s="50"/>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A29" s="49"/>
-      <c r="B29" s="74"/>
-      <c r="C29" s="74"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74"/>
-      <c r="G29" s="74"/>
-      <c r="H29" s="50"/>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A30" s="49"/>
-      <c r="B30" s="74"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="74"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="74"/>
-      <c r="H30" s="50"/>
-      <c r="R30">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A20" s="51"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="73"/>
+      <c r="D20" s="73"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="73"/>
+      <c r="G20" s="73"/>
+      <c r="H20" s="73"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="50"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A21" s="51"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="73"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="73"/>
+      <c r="G21" s="73"/>
+      <c r="H21" s="73"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="50"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A22" s="51"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="73"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="50"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A23" s="51"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="73"/>
+      <c r="H23" s="73"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="50"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A24" s="51"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="73"/>
+      <c r="D24" s="73"/>
+      <c r="E24" s="73"/>
+      <c r="F24" s="73"/>
+      <c r="G24" s="73"/>
+      <c r="H24" s="73"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="50"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A25" s="51"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="73"/>
+      <c r="H25" s="73"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="50"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A26" s="51"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="73"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="73"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="73"/>
+      <c r="H26" s="73"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="50"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A27" s="51"/>
+      <c r="B27" s="48"/>
+      <c r="C27" s="73"/>
+      <c r="D27" s="73"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="73"/>
+      <c r="H27" s="73"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="50"/>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A28" s="51"/>
+      <c r="B28" s="48"/>
+      <c r="C28" s="73"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="73"/>
+      <c r="G28" s="73"/>
+      <c r="H28" s="73"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="50"/>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A29" s="51"/>
+      <c r="B29" s="48"/>
+      <c r="C29" s="73"/>
+      <c r="D29" s="73"/>
+      <c r="E29" s="73"/>
+      <c r="F29" s="73"/>
+      <c r="G29" s="73"/>
+      <c r="H29" s="73"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="50"/>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A30" s="51"/>
+      <c r="B30" s="48"/>
+      <c r="C30" s="73"/>
+      <c r="D30" s="73"/>
+      <c r="E30" s="73"/>
+      <c r="F30" s="73"/>
+      <c r="G30" s="73"/>
+      <c r="H30" s="73"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="50"/>
+      <c r="S30">
         <v>33547.5</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A31" s="49"/>
-      <c r="B31" s="74"/>
-      <c r="C31" s="74"/>
-      <c r="D31" s="74"/>
-      <c r="E31" s="74"/>
-      <c r="F31" s="74"/>
-      <c r="G31" s="74"/>
-      <c r="H31" s="50"/>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A32" s="49"/>
-      <c r="B32" s="74"/>
-      <c r="C32" s="74"/>
-      <c r="D32" s="74"/>
-      <c r="E32" s="74"/>
-      <c r="F32" s="74"/>
-      <c r="G32" s="74"/>
-      <c r="H32" s="50"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A33" s="49"/>
-      <c r="B33" s="74"/>
-      <c r="C33" s="74"/>
-      <c r="D33" s="74"/>
-      <c r="E33" s="74"/>
-      <c r="F33" s="74"/>
-      <c r="G33" s="74"/>
-      <c r="H33" s="50"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A34" s="49"/>
-      <c r="B34" s="74"/>
-      <c r="C34" s="74"/>
-      <c r="D34" s="74"/>
-      <c r="E34" s="74"/>
-      <c r="F34" s="74"/>
-      <c r="G34" s="74"/>
-      <c r="H34" s="50"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A35" s="49"/>
-      <c r="B35" s="74"/>
-      <c r="C35" s="74"/>
-      <c r="D35" s="74"/>
-      <c r="E35" s="74"/>
-      <c r="F35" s="74"/>
-      <c r="G35" s="74"/>
-      <c r="H35" s="50"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A36" s="49"/>
-      <c r="B36" s="74"/>
-      <c r="C36" s="74"/>
-      <c r="D36" s="74"/>
-      <c r="E36" s="74"/>
-      <c r="F36" s="74"/>
-      <c r="G36" s="74"/>
-      <c r="H36" s="50"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A37" s="49"/>
-      <c r="B37" s="74"/>
-      <c r="C37" s="74"/>
-      <c r="D37" s="74"/>
-      <c r="E37" s="74"/>
-      <c r="F37" s="74"/>
-      <c r="G37" s="74"/>
-      <c r="H37" s="50"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A38" s="49"/>
-      <c r="B38" s="74"/>
-      <c r="C38" s="74"/>
-      <c r="D38" s="74"/>
-      <c r="E38" s="74"/>
-      <c r="F38" s="74"/>
-      <c r="G38" s="75"/>
-      <c r="H38" s="76"/>
-    </row>
-    <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="2"/>
-      <c r="B39" s="3"/>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A31" s="51"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="73"/>
+      <c r="D31" s="73"/>
+      <c r="E31" s="73"/>
+      <c r="F31" s="73"/>
+      <c r="G31" s="73"/>
+      <c r="H31" s="73"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="50"/>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A32" s="51"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="73"/>
+      <c r="D32" s="73"/>
+      <c r="E32" s="73"/>
+      <c r="F32" s="73"/>
+      <c r="G32" s="73"/>
+      <c r="H32" s="73"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="50"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A33" s="51"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="73"/>
+      <c r="D33" s="73"/>
+      <c r="E33" s="73"/>
+      <c r="F33" s="73"/>
+      <c r="G33" s="73"/>
+      <c r="H33" s="73"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="50"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A34" s="51"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="73"/>
+      <c r="D34" s="73"/>
+      <c r="E34" s="73"/>
+      <c r="F34" s="73"/>
+      <c r="G34" s="73"/>
+      <c r="H34" s="73"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="50"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A35" s="51"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="73"/>
+      <c r="D35" s="73"/>
+      <c r="E35" s="73"/>
+      <c r="F35" s="73"/>
+      <c r="G35" s="73"/>
+      <c r="H35" s="73"/>
+      <c r="I35" s="49"/>
+      <c r="J35" s="50"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A36" s="51"/>
+      <c r="B36" s="48"/>
+      <c r="C36" s="73"/>
+      <c r="D36" s="73"/>
+      <c r="E36" s="73"/>
+      <c r="F36" s="73"/>
+      <c r="G36" s="73"/>
+      <c r="H36" s="73"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="50"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A37" s="51"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="73"/>
+      <c r="D37" s="73"/>
+      <c r="E37" s="73"/>
+      <c r="F37" s="73"/>
+      <c r="G37" s="73"/>
+      <c r="H37" s="73"/>
+      <c r="I37" s="49"/>
+      <c r="J37" s="50"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A38" s="51"/>
+      <c r="B38" s="48"/>
+      <c r="C38" s="73"/>
+      <c r="D38" s="73"/>
+      <c r="E38" s="73"/>
+      <c r="F38" s="73"/>
+      <c r="G38" s="73"/>
+      <c r="H38" s="74"/>
+      <c r="I38" s="75"/>
+      <c r="J38" s="50"/>
+    </row>
+    <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="51"/>
+      <c r="B39" s="2"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
-      <c r="H39" s="4"/>
-    </row>
-    <row r="40" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="2" t="s">
+      <c r="H39" s="3"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="50"/>
+    </row>
+    <row r="40" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="51"/>
+      <c r="B40" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
-      <c r="H40" s="4"/>
-    </row>
-    <row r="41" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="77" t="s">
+      <c r="H40" s="3"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="50"/>
+    </row>
+    <row r="41" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="51"/>
+      <c r="B41" s="76" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="78"/>
-      <c r="C41" s="78"/>
-      <c r="D41" s="78"/>
-      <c r="E41" s="78"/>
-      <c r="F41" s="78"/>
-      <c r="G41" s="78"/>
-      <c r="H41" s="79"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A42" s="61"/>
-      <c r="B42" s="40"/>
-      <c r="C42" s="80" t="s">
+      <c r="C41" s="77"/>
+      <c r="D41" s="77"/>
+      <c r="E41" s="77"/>
+      <c r="F41" s="77"/>
+      <c r="G41" s="77"/>
+      <c r="H41" s="77"/>
+      <c r="I41" s="78"/>
+      <c r="J41" s="50"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A42" s="51"/>
+      <c r="B42" s="60"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="D42" s="80" t="s">
+      <c r="E42" s="79" t="s">
         <v>161</v>
       </c>
-      <c r="E42" s="81" t="s">
+      <c r="F42" s="80" t="s">
         <v>162</v>
       </c>
-      <c r="G42" s="82"/>
-      <c r="H42" s="83" t="s">
+      <c r="H42" s="81"/>
+      <c r="I42" s="82" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A43" s="123" t="s">
+      <c r="J42" s="50"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A43" s="51"/>
+      <c r="B43" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="B43" s="124"/>
-      <c r="C43" s="124"/>
-      <c r="D43" s="124"/>
-      <c r="E43" s="124"/>
-      <c r="F43" s="124"/>
-      <c r="G43" s="82"/>
-      <c r="H43" s="66"/>
-    </row>
-    <row r="44" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="84" t="s">
+      <c r="C43" s="122"/>
+      <c r="D43" s="122"/>
+      <c r="E43" s="122"/>
+      <c r="F43" s="122"/>
+      <c r="G43" s="122"/>
+      <c r="H43" s="81"/>
+      <c r="I43" s="65"/>
+      <c r="J43" s="50"/>
+    </row>
+    <row r="44" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="51"/>
+      <c r="B44" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="85"/>
-      <c r="C44" s="85"/>
-      <c r="D44" s="85"/>
-      <c r="E44" s="53" t="s">
+      <c r="C44" s="84"/>
+      <c r="D44" s="84"/>
+      <c r="E44" s="84"/>
+      <c r="F44" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="F44" s="54"/>
-      <c r="G44" s="54"/>
-      <c r="H44" s="56"/>
-    </row>
-    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="47" t="s">
+      <c r="G44" s="53"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="55"/>
+      <c r="J44" s="50"/>
+    </row>
+    <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="51"/>
+      <c r="B45" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="48"/>
-      <c r="C45" s="48"/>
-      <c r="D45" s="48"/>
-      <c r="E45" s="51"/>
-      <c r="H45" s="52"/>
-    </row>
-    <row r="46" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="47" t="s">
+      <c r="C45" s="47"/>
+      <c r="D45" s="47"/>
+      <c r="E45" s="47"/>
+      <c r="F45" s="50"/>
+      <c r="I45" s="51"/>
+      <c r="J45" s="50"/>
+    </row>
+    <row r="46" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="51"/>
+      <c r="B46" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="48"/>
-      <c r="C46" s="48"/>
-      <c r="D46" s="48"/>
-      <c r="E46" s="51"/>
-      <c r="H46" s="52"/>
-    </row>
-    <row r="47" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="47" t="s">
+      <c r="C46" s="47"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="47"/>
+      <c r="F46" s="50"/>
+      <c r="I46" s="51"/>
+      <c r="J46" s="50"/>
+    </row>
+    <row r="47" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="51"/>
+      <c r="B47" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="B47" s="48"/>
-      <c r="C47" s="48"/>
-      <c r="D47" s="48"/>
-      <c r="E47" s="51"/>
-      <c r="H47" s="52"/>
-    </row>
-    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="71" t="s">
+      <c r="C47" s="47"/>
+      <c r="D47" s="47"/>
+      <c r="E47" s="47"/>
+      <c r="F47" s="50"/>
+      <c r="I47" s="51"/>
+      <c r="J47" s="50"/>
+    </row>
+    <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="51"/>
+      <c r="B48" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="B48" s="72"/>
-      <c r="C48" s="72"/>
-      <c r="D48" s="73"/>
-      <c r="E48" s="86"/>
-      <c r="F48" s="69"/>
-      <c r="G48" s="69"/>
-      <c r="H48" s="70"/>
-    </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="45"/>
-      <c r="B49" s="45"/>
-      <c r="C49" s="45"/>
-      <c r="D49" s="45"/>
-    </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="45"/>
-      <c r="B50" s="45"/>
-      <c r="C50" s="45"/>
-      <c r="D50" s="45"/>
-    </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="45"/>
-      <c r="B51" s="45"/>
-      <c r="C51" s="45"/>
-      <c r="D51" s="45"/>
-    </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="45"/>
-      <c r="B52" s="45"/>
-      <c r="C52" s="45"/>
-      <c r="D52" s="45"/>
-    </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="45"/>
-      <c r="B53" s="45"/>
-      <c r="C53" s="45"/>
-      <c r="D53" s="45"/>
-    </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="45"/>
-      <c r="B54" s="45"/>
-      <c r="C54" s="45"/>
-      <c r="D54" s="45"/>
-    </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="45"/>
-      <c r="B55" s="45"/>
-      <c r="C55" s="45"/>
-      <c r="D55" s="45"/>
-    </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="45"/>
-      <c r="B56" s="45"/>
-      <c r="C56" s="45"/>
-      <c r="D56" s="45"/>
-    </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="45"/>
-      <c r="B57" s="45"/>
-      <c r="C57" s="45"/>
-      <c r="D57" s="45"/>
-    </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="45"/>
-      <c r="B58" s="45"/>
-      <c r="C58" s="45"/>
-      <c r="D58" s="45"/>
-    </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="45"/>
-      <c r="B59" s="45"/>
-      <c r="C59" s="45"/>
-      <c r="D59" s="45"/>
-    </row>
-    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="45"/>
-      <c r="B60" s="45"/>
-      <c r="C60" s="45"/>
-      <c r="D60" s="45"/>
-    </row>
-    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="45"/>
-      <c r="B61" s="45"/>
-      <c r="C61" s="45"/>
-      <c r="D61" s="45"/>
-    </row>
-    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="45"/>
-      <c r="B62" s="45"/>
-      <c r="C62" s="45"/>
-      <c r="D62" s="45"/>
-    </row>
-    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="45"/>
-      <c r="B63" s="45"/>
-      <c r="C63" s="45"/>
-      <c r="D63" s="45"/>
-    </row>
-    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A64" s="45"/>
-      <c r="B64" s="45"/>
-      <c r="C64" s="45"/>
-      <c r="D64" s="45"/>
-    </row>
-    <row r="65" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A65" s="45"/>
-      <c r="B65" s="45"/>
-      <c r="C65" s="45"/>
-      <c r="D65" s="45"/>
-    </row>
-    <row r="66" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A66" s="45"/>
-      <c r="B66" s="45"/>
-      <c r="C66" s="45"/>
-      <c r="D66" s="45"/>
-    </row>
-    <row r="67" spans="1:8" ht="28.15" customHeight="1" x14ac:dyDescent="0.85">
-      <c r="A67" s="107" t="s">
+      <c r="C48" s="71"/>
+      <c r="D48" s="71"/>
+      <c r="E48" s="72"/>
+      <c r="F48" s="85"/>
+      <c r="G48" s="68"/>
+      <c r="H48" s="68"/>
+      <c r="I48" s="69"/>
+      <c r="J48" s="50"/>
+    </row>
+    <row r="49" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B49" s="44"/>
+      <c r="C49" s="44"/>
+      <c r="D49" s="44"/>
+      <c r="E49" s="44"/>
+    </row>
+    <row r="50" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B50" s="44"/>
+      <c r="C50" s="44"/>
+      <c r="D50" s="44"/>
+      <c r="E50" s="44"/>
+    </row>
+    <row r="51" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B51" s="44"/>
+      <c r="C51" s="44"/>
+      <c r="D51" s="44"/>
+      <c r="E51" s="44"/>
+    </row>
+    <row r="52" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B52" s="44"/>
+      <c r="C52" s="44"/>
+      <c r="D52" s="44"/>
+      <c r="E52" s="44"/>
+    </row>
+    <row r="53" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B53" s="44"/>
+      <c r="C53" s="44"/>
+      <c r="D53" s="44"/>
+      <c r="E53" s="44"/>
+    </row>
+    <row r="54" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B54" s="44"/>
+      <c r="C54" s="44"/>
+      <c r="D54" s="44"/>
+      <c r="E54" s="44"/>
+    </row>
+    <row r="55" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B55" s="44"/>
+      <c r="C55" s="44"/>
+      <c r="D55" s="44"/>
+      <c r="E55" s="44"/>
+    </row>
+    <row r="56" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B56" s="44"/>
+      <c r="C56" s="44"/>
+      <c r="D56" s="44"/>
+      <c r="E56" s="44"/>
+    </row>
+    <row r="57" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B57" s="44"/>
+      <c r="C57" s="44"/>
+      <c r="D57" s="44"/>
+      <c r="E57" s="44"/>
+    </row>
+    <row r="58" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B58" s="44"/>
+      <c r="C58" s="44"/>
+      <c r="D58" s="44"/>
+      <c r="E58" s="44"/>
+    </row>
+    <row r="59" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B59" s="44"/>
+      <c r="C59" s="44"/>
+      <c r="D59" s="44"/>
+      <c r="E59" s="44"/>
+    </row>
+    <row r="60" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B60" s="44"/>
+      <c r="C60" s="44"/>
+      <c r="D60" s="44"/>
+      <c r="E60" s="44"/>
+    </row>
+    <row r="61" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B61" s="44"/>
+      <c r="C61" s="44"/>
+      <c r="D61" s="44"/>
+      <c r="E61" s="44"/>
+    </row>
+    <row r="62" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B62" s="44"/>
+      <c r="C62" s="44"/>
+      <c r="D62" s="44"/>
+      <c r="E62" s="44"/>
+    </row>
+    <row r="63" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B63" s="44"/>
+      <c r="C63" s="44"/>
+      <c r="D63" s="44"/>
+      <c r="E63" s="44"/>
+    </row>
+    <row r="64" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B64" s="44"/>
+      <c r="C64" s="44"/>
+      <c r="D64" s="44"/>
+      <c r="E64" s="44"/>
+    </row>
+    <row r="65" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B65" s="44"/>
+      <c r="C65" s="44"/>
+      <c r="D65" s="44"/>
+      <c r="E65" s="44"/>
+    </row>
+    <row r="66" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B66" s="44"/>
+      <c r="C66" s="44"/>
+      <c r="D66" s="44"/>
+      <c r="E66" s="44"/>
+    </row>
+    <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B67" s="44"/>
+      <c r="C67" s="44"/>
+      <c r="D67" s="44"/>
+      <c r="E67" s="44"/>
+    </row>
+    <row r="68" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B68" s="44"/>
+      <c r="C68" s="44"/>
+      <c r="D68" s="44"/>
+      <c r="E68" s="44"/>
+    </row>
+    <row r="69" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B69" s="44"/>
+      <c r="C69" s="44"/>
+      <c r="D69" s="44"/>
+      <c r="E69" s="44"/>
+    </row>
+    <row r="70" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B70" s="44"/>
+      <c r="C70" s="44"/>
+      <c r="D70" s="44"/>
+      <c r="E70" s="44"/>
+    </row>
+    <row r="71" spans="1:10" ht="28.15" customHeight="1" x14ac:dyDescent="0.85">
+      <c r="B71" s="104" t="s">
         <v>56</v>
       </c>
-      <c r="B67" s="87"/>
-      <c r="C67" s="87"/>
-      <c r="D67" s="87"/>
-      <c r="E67" s="87"/>
-      <c r="F67" s="87"/>
-      <c r="G67" s="87"/>
-      <c r="H67" s="87"/>
-    </row>
-    <row r="68" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A68" s="88" t="s">
+      <c r="C71" s="86"/>
+      <c r="D71" s="86"/>
+      <c r="E71" s="86"/>
+      <c r="F71" s="86"/>
+      <c r="G71" s="86"/>
+      <c r="H71" s="86"/>
+      <c r="I71" s="86"/>
+    </row>
+    <row r="72" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A72" s="51"/>
+      <c r="B72" s="126" t="s">
         <v>57</v>
       </c>
-      <c r="B68" s="89"/>
-      <c r="C68" s="89"/>
-      <c r="D68" s="89"/>
-      <c r="E68" s="88" t="s">
+      <c r="C72" s="88"/>
+      <c r="D72" s="88"/>
+      <c r="E72" s="88"/>
+      <c r="F72" s="87" t="s">
         <v>58</v>
       </c>
-      <c r="F68" s="89"/>
-      <c r="G68" s="90" t="s">
+      <c r="G72" s="88"/>
+      <c r="H72" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="H68" s="91" t="s">
+      <c r="I72" s="90" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A69" s="59" t="s">
+      <c r="J72" s="50"/>
+    </row>
+    <row r="73" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A73" s="51"/>
+      <c r="B73" s="127" t="s">
         <v>59</v>
       </c>
-      <c r="B69" s="45"/>
-      <c r="C69" s="45"/>
-      <c r="D69" s="45"/>
-      <c r="E69" s="47" t="s">
+      <c r="C73" s="44"/>
+      <c r="D73" s="44"/>
+      <c r="E73" s="44"/>
+      <c r="F73" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="F69" s="48"/>
-      <c r="G69" s="92" t="s">
+      <c r="G73" s="47"/>
+      <c r="H73" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="H69" s="76" t="s">
+      <c r="I73" s="75" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A70" s="71" t="s">
+      <c r="J73" s="50"/>
+    </row>
+    <row r="74" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A74" s="51"/>
+      <c r="B74" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="B70" s="72"/>
-      <c r="C70" s="72"/>
-      <c r="D70" s="45"/>
-      <c r="E70" s="59"/>
-      <c r="F70" s="45"/>
-      <c r="G70" s="51"/>
-      <c r="H70" s="52"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A71" s="93" t="s">
+      <c r="C74" s="71"/>
+      <c r="D74" s="71"/>
+      <c r="E74" s="44"/>
+      <c r="F74" s="58"/>
+      <c r="G74" s="44"/>
+      <c r="H74" s="50"/>
+      <c r="I74" s="51"/>
+      <c r="J74" s="50"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A75" s="51"/>
+      <c r="B75" s="92" t="s">
         <v>62</v>
       </c>
-      <c r="B71" s="89"/>
-      <c r="C71" s="89"/>
-      <c r="D71" s="94"/>
-      <c r="E71" s="53" t="s">
+      <c r="C75" s="88"/>
+      <c r="D75" s="88"/>
+      <c r="E75" s="92"/>
+      <c r="F75" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="F71" s="54"/>
-      <c r="G71" s="54"/>
-      <c r="H71" s="56"/>
-    </row>
-    <row r="72" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A72" s="47" t="s">
+      <c r="G75" s="53"/>
+      <c r="H75" s="53"/>
+      <c r="I75" s="55"/>
+      <c r="J75" s="50"/>
+    </row>
+    <row r="76" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A76" s="51"/>
+      <c r="B76" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="B72" s="48"/>
-      <c r="C72" s="48"/>
-      <c r="D72" s="48"/>
-      <c r="E72" s="59" t="s">
+      <c r="C76" s="47"/>
+      <c r="D76" s="47"/>
+      <c r="E76" s="47"/>
+      <c r="F76" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="F72" s="45"/>
-      <c r="G72" s="45"/>
-      <c r="H72" s="60"/>
-    </row>
-    <row r="73" spans="1:8" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A73" s="116" t="s">
+      <c r="G76" s="44"/>
+      <c r="H76" s="44"/>
+      <c r="I76" s="59"/>
+      <c r="J76" s="50"/>
+    </row>
+    <row r="77" spans="1:10" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A77" s="51"/>
+      <c r="B77" s="115" t="s">
         <v>15</v>
       </c>
-      <c r="B73" s="117"/>
-      <c r="C73" s="117"/>
-      <c r="D73" s="118"/>
-      <c r="E73" s="116" t="s">
+      <c r="C77" s="115"/>
+      <c r="D77" s="115"/>
+      <c r="E77" s="116"/>
+      <c r="F77" s="114" t="s">
         <v>146</v>
       </c>
-      <c r="F73" s="117"/>
-      <c r="G73" s="117"/>
-      <c r="H73" s="118"/>
-    </row>
-    <row r="74" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A74" s="95" t="s">
+      <c r="G77" s="115"/>
+      <c r="H77" s="115"/>
+      <c r="I77" s="116"/>
+      <c r="J77" s="50"/>
+    </row>
+    <row r="78" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A78" s="51"/>
+      <c r="B78" s="129" t="s">
         <v>64</v>
       </c>
-      <c r="B74" s="64" t="s">
+      <c r="C78" s="63" t="s">
         <v>156</v>
       </c>
-      <c r="D74" s="52"/>
-      <c r="E74" s="53" t="s">
+      <c r="E78" s="51"/>
+      <c r="F78" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="F74" s="54"/>
-      <c r="G74" s="54"/>
-      <c r="H74" s="56"/>
-    </row>
-    <row r="75" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A75" s="59" t="s">
+      <c r="G78" s="53"/>
+      <c r="H78" s="53"/>
+      <c r="I78" s="55"/>
+      <c r="J78" s="50"/>
+    </row>
+    <row r="79" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A79" s="51"/>
+      <c r="B79" s="127" t="s">
         <v>66</v>
       </c>
-      <c r="B75" s="96" t="s">
+      <c r="C79" s="93" t="s">
         <v>67</v>
       </c>
-      <c r="D75" s="52"/>
-      <c r="E75" s="39" t="s">
+      <c r="E79" s="51"/>
+      <c r="F79" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="F75" s="64"/>
-      <c r="G75" s="64"/>
-      <c r="H75" s="65"/>
-    </row>
-    <row r="76" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A76" s="95" t="s">
+      <c r="G79" s="63"/>
+      <c r="H79" s="63"/>
+      <c r="I79" s="64"/>
+      <c r="J79" s="50"/>
+    </row>
+    <row r="80" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A80" s="51"/>
+      <c r="B80" s="129" t="s">
         <v>69</v>
       </c>
-      <c r="B76" s="97" t="s">
+      <c r="C80" s="94" t="s">
         <v>70</v>
       </c>
-      <c r="D76" s="66"/>
-      <c r="E76" s="59" t="s">
+      <c r="E80" s="65"/>
+      <c r="F80" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="F76" s="45"/>
-      <c r="G76" s="45"/>
-      <c r="H76" s="60"/>
-    </row>
-    <row r="77" spans="1:8" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A77" s="67" t="s">
+      <c r="G80" s="44"/>
+      <c r="H80" s="44"/>
+      <c r="I80" s="59"/>
+      <c r="J80" s="50"/>
+    </row>
+    <row r="81" spans="1:18" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A81" s="51"/>
+      <c r="B81" s="67" t="s">
         <v>155</v>
       </c>
-      <c r="B77" s="72" t="s">
+      <c r="C81" s="71" t="s">
         <v>72</v>
       </c>
-      <c r="D77" s="70"/>
-      <c r="E77" s="71" t="s">
+      <c r="E81" s="69"/>
+      <c r="F81" s="70" t="s">
         <v>73</v>
       </c>
-      <c r="F77" s="72"/>
-      <c r="G77" s="72"/>
-      <c r="H77" s="73"/>
-    </row>
-    <row r="78" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A78" s="51" t="s">
+      <c r="G81" s="71"/>
+      <c r="H81" s="71"/>
+      <c r="I81" s="72"/>
+      <c r="J81" s="50"/>
+    </row>
+    <row r="82" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A82" s="51"/>
+      <c r="B82" s="130" t="s">
         <v>154</v>
       </c>
-      <c r="C78" s="98"/>
-      <c r="D78" s="66"/>
-      <c r="E78" s="53" t="s">
+      <c r="D82" s="95"/>
+      <c r="E82" s="65"/>
+      <c r="F82" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="F78" s="54"/>
-      <c r="G78" s="54"/>
-      <c r="H78" s="56"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A79" s="51"/>
-      <c r="C79" s="69"/>
-      <c r="D79" s="99"/>
-      <c r="E79" s="71" t="s">
+      <c r="G82" s="53"/>
+      <c r="H82" s="53"/>
+      <c r="I82" s="55"/>
+      <c r="J82" s="50"/>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A83" s="51"/>
+      <c r="B83" s="130"/>
+      <c r="D83" s="68"/>
+      <c r="E83" s="96"/>
+      <c r="F83" s="70" t="s">
         <v>75</v>
       </c>
-      <c r="F79" s="72"/>
-      <c r="G79" s="72"/>
-      <c r="H79" s="73"/>
-    </row>
-    <row r="80" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A80" s="100" t="s">
+      <c r="G83" s="71"/>
+      <c r="H83" s="71"/>
+      <c r="I83" s="72"/>
+      <c r="J83" s="50"/>
+    </row>
+    <row r="84" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A84" s="51"/>
+      <c r="B84" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="B80" s="101" t="s">
+      <c r="C84" s="98" t="s">
         <v>157</v>
       </c>
-      <c r="C80" s="101" t="s">
+      <c r="D84" s="98" t="s">
         <v>76</v>
       </c>
-      <c r="D80" s="101" t="s">
+      <c r="E84" s="98" t="s">
         <v>77</v>
       </c>
-      <c r="E80" s="102" t="s">
+      <c r="F84" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="F80" s="102"/>
-      <c r="G80" s="101" t="s">
+      <c r="G84" s="99"/>
+      <c r="H84" s="98" t="s">
         <v>79</v>
       </c>
-      <c r="H80" s="103" t="s">
+      <c r="I84" s="100" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="81" spans="1:17" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A81" s="49" t="s">
+      <c r="J84" s="50"/>
+    </row>
+    <row r="85" spans="1:18" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A85" s="51"/>
+      <c r="B85" s="131" t="s">
         <v>35</v>
       </c>
-      <c r="B81" s="74" t="s">
+      <c r="C85" s="73" t="s">
         <v>86</v>
       </c>
-      <c r="C81" s="74" t="s">
+      <c r="D85" s="73" t="s">
         <v>104</v>
       </c>
-      <c r="D81" s="74" t="s">
+      <c r="E85" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="E81" s="74" t="s">
+      <c r="F85" s="73" t="s">
         <v>82</v>
       </c>
-      <c r="F81" s="74" t="s">
+      <c r="G85" s="73" t="s">
         <v>83</v>
       </c>
-      <c r="G81" s="74" t="s">
+      <c r="H85" s="73" t="s">
         <v>84</v>
       </c>
-      <c r="H81" s="50" t="s">
+      <c r="I85" s="49" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="82" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A82" s="49"/>
-      <c r="B82" s="74"/>
-      <c r="C82" s="74"/>
-      <c r="D82" s="74"/>
-      <c r="E82" s="74"/>
-      <c r="F82" s="74"/>
-      <c r="G82" s="74"/>
-      <c r="H82" s="50"/>
-    </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A83" s="49"/>
-      <c r="B83" s="74"/>
-      <c r="C83" s="74"/>
-      <c r="D83" s="74"/>
-      <c r="E83" s="74"/>
-      <c r="F83" s="74"/>
-      <c r="G83" s="74"/>
-      <c r="H83" s="50"/>
-    </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A84" s="49"/>
-      <c r="B84" s="74"/>
-      <c r="C84" s="74"/>
-      <c r="D84" s="74"/>
-      <c r="E84" s="74"/>
-      <c r="F84" s="74"/>
-      <c r="G84" s="74"/>
-      <c r="H84" s="50"/>
-    </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="F85" s="74"/>
-      <c r="G85" s="74"/>
-      <c r="H85" s="50"/>
-    </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A86" s="49"/>
-      <c r="B86" s="74"/>
-      <c r="C86" s="74"/>
-      <c r="D86" s="74"/>
-      <c r="E86" s="74"/>
-      <c r="F86" s="74"/>
-      <c r="G86" s="74"/>
-      <c r="H86" s="50"/>
-      <c r="Q86" s="104"/>
-    </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A87" s="49"/>
-      <c r="B87" s="74"/>
-      <c r="C87" s="74"/>
-      <c r="D87" s="74"/>
-      <c r="E87" s="74"/>
-      <c r="F87" s="74"/>
-      <c r="G87" s="74"/>
-      <c r="H87" s="50"/>
-    </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A88" s="49"/>
-      <c r="B88" s="74"/>
-      <c r="C88" s="74"/>
-      <c r="D88" s="74"/>
-      <c r="E88" s="74"/>
-      <c r="F88" s="74"/>
-      <c r="G88" s="74"/>
-      <c r="H88" s="50"/>
-    </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A89" s="49"/>
-      <c r="B89" s="74"/>
-      <c r="C89" s="74"/>
-      <c r="D89" s="74"/>
-      <c r="E89" s="74"/>
-      <c r="F89" s="74"/>
-      <c r="G89" s="74"/>
-      <c r="H89" s="50"/>
-    </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A90" s="49"/>
-      <c r="B90" s="74"/>
-      <c r="C90" s="74"/>
-      <c r="D90" s="74"/>
-      <c r="E90" s="74"/>
-      <c r="F90" s="74"/>
-      <c r="G90" s="74"/>
-      <c r="H90" s="50"/>
-    </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A91" s="49"/>
-      <c r="B91" s="74"/>
-      <c r="C91" s="74"/>
-      <c r="D91" s="74"/>
-      <c r="E91" s="74"/>
-      <c r="F91" s="74"/>
-      <c r="G91" s="74"/>
-      <c r="H91" s="50"/>
-    </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A92" s="49"/>
-      <c r="B92" s="74"/>
-      <c r="C92" s="74"/>
-      <c r="D92" s="74"/>
-      <c r="E92" s="74"/>
-      <c r="F92" s="74"/>
-      <c r="G92" s="74"/>
-      <c r="H92" s="50"/>
-    </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A93" s="49"/>
-      <c r="B93" s="74"/>
-      <c r="C93" s="74"/>
-      <c r="D93" s="74"/>
-      <c r="E93" s="74"/>
-      <c r="F93" s="74"/>
-      <c r="G93" s="74"/>
-      <c r="H93" s="50"/>
-    </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A94" s="49"/>
-      <c r="B94" s="74"/>
-      <c r="C94" s="74"/>
-      <c r="D94" s="74"/>
-      <c r="E94" s="74"/>
-      <c r="F94" s="74"/>
-      <c r="G94" s="74"/>
-      <c r="H94" s="50"/>
-    </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A95" s="49"/>
-      <c r="B95" s="74"/>
-      <c r="C95" s="74"/>
-      <c r="D95" s="74"/>
-      <c r="E95" s="74"/>
-      <c r="F95" s="74"/>
-      <c r="G95" s="74"/>
-      <c r="H95" s="50"/>
-    </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A96" s="49"/>
-      <c r="B96" s="74"/>
-      <c r="C96" s="74"/>
-      <c r="D96" s="74"/>
-      <c r="E96" s="74"/>
-      <c r="F96" s="74"/>
-      <c r="G96" s="74"/>
-      <c r="H96" s="50"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A97" s="49"/>
-      <c r="B97" s="74"/>
-      <c r="C97" s="74"/>
-      <c r="D97" s="74"/>
-      <c r="E97" s="74"/>
-      <c r="G97" s="74"/>
-      <c r="H97" s="50"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A98" s="49"/>
-      <c r="B98" s="74"/>
-      <c r="C98" s="74"/>
-      <c r="D98" s="74"/>
-      <c r="E98" s="74"/>
-      <c r="F98" s="74"/>
-      <c r="G98" s="74"/>
-      <c r="H98" s="50"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A99" s="49"/>
-      <c r="B99" s="74"/>
-      <c r="C99" s="74"/>
-      <c r="D99" s="74"/>
-      <c r="E99" s="74"/>
-      <c r="F99" s="74"/>
-      <c r="G99" s="74"/>
-      <c r="H99" s="50"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A100" s="49"/>
-      <c r="B100" s="74"/>
-      <c r="C100" s="74"/>
-      <c r="D100" s="74"/>
-      <c r="E100" s="74"/>
-      <c r="F100" s="74"/>
-      <c r="G100" s="74"/>
-      <c r="H100" s="50"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A101" s="49"/>
-      <c r="B101" s="74"/>
-      <c r="C101" s="74"/>
-      <c r="D101" s="74"/>
-      <c r="E101" s="74"/>
-      <c r="F101" s="74"/>
-      <c r="G101" s="74"/>
-      <c r="H101" s="50"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A102" s="62"/>
-      <c r="B102" s="46"/>
-      <c r="C102" s="46"/>
-      <c r="D102" s="46"/>
-      <c r="E102" s="46"/>
-      <c r="F102" s="46"/>
-      <c r="G102" s="82"/>
-      <c r="H102" s="66"/>
-    </row>
-    <row r="103" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A103" s="5"/>
-      <c r="B103" s="6"/>
-      <c r="C103" s="6"/>
-      <c r="D103" s="6"/>
-      <c r="E103" s="6"/>
-      <c r="F103" s="6"/>
-      <c r="G103" s="6"/>
-      <c r="H103" s="7"/>
-    </row>
-    <row r="104" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A104" s="2" t="s">
+      <c r="J85" s="50"/>
+    </row>
+    <row r="86" spans="1:18" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A86" s="51"/>
+      <c r="B86" s="131"/>
+      <c r="C86" s="73"/>
+      <c r="D86" s="73"/>
+      <c r="E86" s="73"/>
+      <c r="F86" s="73"/>
+      <c r="G86" s="73"/>
+      <c r="H86" s="73"/>
+      <c r="I86" s="49"/>
+      <c r="J86" s="50"/>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A87" s="51"/>
+      <c r="B87" s="131"/>
+      <c r="C87" s="73"/>
+      <c r="D87" s="73"/>
+      <c r="E87" s="73"/>
+      <c r="F87" s="73"/>
+      <c r="G87" s="73"/>
+      <c r="H87" s="73"/>
+      <c r="I87" s="49"/>
+      <c r="J87" s="50"/>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A88" s="51"/>
+      <c r="B88" s="131"/>
+      <c r="C88" s="73"/>
+      <c r="D88" s="73"/>
+      <c r="E88" s="73"/>
+      <c r="F88" s="73"/>
+      <c r="G88" s="73"/>
+      <c r="H88" s="73"/>
+      <c r="I88" s="49"/>
+      <c r="J88" s="50"/>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A89" s="51"/>
+      <c r="G89" s="73"/>
+      <c r="H89" s="73"/>
+      <c r="I89" s="49"/>
+      <c r="J89" s="50"/>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A90" s="51"/>
+      <c r="B90" s="131"/>
+      <c r="C90" s="73"/>
+      <c r="D90" s="73"/>
+      <c r="E90" s="73"/>
+      <c r="F90" s="73"/>
+      <c r="G90" s="73"/>
+      <c r="H90" s="73"/>
+      <c r="I90" s="49"/>
+      <c r="J90" s="50"/>
+      <c r="R90" s="101"/>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A91" s="51"/>
+      <c r="B91" s="131"/>
+      <c r="C91" s="73"/>
+      <c r="D91" s="73"/>
+      <c r="E91" s="73"/>
+      <c r="F91" s="73"/>
+      <c r="G91" s="73"/>
+      <c r="H91" s="73"/>
+      <c r="I91" s="49"/>
+      <c r="J91" s="50"/>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A92" s="51"/>
+      <c r="B92" s="131"/>
+      <c r="C92" s="73"/>
+      <c r="D92" s="73"/>
+      <c r="E92" s="73"/>
+      <c r="F92" s="73"/>
+      <c r="G92" s="73"/>
+      <c r="H92" s="73"/>
+      <c r="I92" s="49"/>
+      <c r="J92" s="50"/>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A93" s="51"/>
+      <c r="B93" s="131"/>
+      <c r="C93" s="73"/>
+      <c r="D93" s="73"/>
+      <c r="E93" s="73"/>
+      <c r="F93" s="73"/>
+      <c r="G93" s="73"/>
+      <c r="H93" s="73"/>
+      <c r="I93" s="49"/>
+      <c r="J93" s="50"/>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A94" s="51"/>
+      <c r="B94" s="131"/>
+      <c r="C94" s="73"/>
+      <c r="D94" s="73"/>
+      <c r="E94" s="73"/>
+      <c r="F94" s="73"/>
+      <c r="G94" s="73"/>
+      <c r="H94" s="73"/>
+      <c r="I94" s="49"/>
+      <c r="J94" s="50"/>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A95" s="51"/>
+      <c r="B95" s="131"/>
+      <c r="C95" s="73"/>
+      <c r="D95" s="73"/>
+      <c r="E95" s="73"/>
+      <c r="F95" s="73"/>
+      <c r="G95" s="73"/>
+      <c r="H95" s="73"/>
+      <c r="I95" s="49"/>
+      <c r="J95" s="50"/>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A96" s="51"/>
+      <c r="B96" s="131"/>
+      <c r="C96" s="73"/>
+      <c r="D96" s="73"/>
+      <c r="E96" s="73"/>
+      <c r="F96" s="73"/>
+      <c r="G96" s="73"/>
+      <c r="H96" s="73"/>
+      <c r="I96" s="49"/>
+      <c r="J96" s="50"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A97" s="51"/>
+      <c r="B97" s="131"/>
+      <c r="C97" s="73"/>
+      <c r="D97" s="73"/>
+      <c r="E97" s="73"/>
+      <c r="F97" s="73"/>
+      <c r="G97" s="73"/>
+      <c r="H97" s="73"/>
+      <c r="I97" s="49"/>
+      <c r="J97" s="50"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A98" s="51"/>
+      <c r="B98" s="131"/>
+      <c r="C98" s="73"/>
+      <c r="D98" s="73"/>
+      <c r="E98" s="73"/>
+      <c r="F98" s="73"/>
+      <c r="G98" s="73"/>
+      <c r="H98" s="73"/>
+      <c r="I98" s="49"/>
+      <c r="J98" s="50"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A99" s="51"/>
+      <c r="B99" s="131"/>
+      <c r="C99" s="73"/>
+      <c r="D99" s="73"/>
+      <c r="E99" s="73"/>
+      <c r="F99" s="73"/>
+      <c r="G99" s="73"/>
+      <c r="H99" s="73"/>
+      <c r="I99" s="49"/>
+      <c r="J99" s="50"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A100" s="51"/>
+      <c r="B100" s="131"/>
+      <c r="C100" s="73"/>
+      <c r="D100" s="73"/>
+      <c r="E100" s="73"/>
+      <c r="F100" s="73"/>
+      <c r="G100" s="73"/>
+      <c r="H100" s="73"/>
+      <c r="I100" s="49"/>
+      <c r="J100" s="50"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A101" s="51"/>
+      <c r="B101" s="131"/>
+      <c r="C101" s="73"/>
+      <c r="D101" s="73"/>
+      <c r="E101" s="73"/>
+      <c r="F101" s="73"/>
+      <c r="H101" s="73"/>
+      <c r="I101" s="49"/>
+      <c r="J101" s="50"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A102" s="51"/>
+      <c r="B102" s="131"/>
+      <c r="C102" s="73"/>
+      <c r="D102" s="73"/>
+      <c r="E102" s="73"/>
+      <c r="F102" s="73"/>
+      <c r="G102" s="73"/>
+      <c r="H102" s="73"/>
+      <c r="I102" s="49"/>
+      <c r="J102" s="50"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A103" s="51"/>
+      <c r="B103" s="131"/>
+      <c r="C103" s="73"/>
+      <c r="D103" s="73"/>
+      <c r="E103" s="73"/>
+      <c r="F103" s="73"/>
+      <c r="G103" s="73"/>
+      <c r="H103" s="73"/>
+      <c r="I103" s="49"/>
+      <c r="J103" s="50"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A104" s="51"/>
+      <c r="B104" s="131"/>
+      <c r="C104" s="73"/>
+      <c r="D104" s="73"/>
+      <c r="E104" s="73"/>
+      <c r="F104" s="73"/>
+      <c r="G104" s="73"/>
+      <c r="H104" s="73"/>
+      <c r="I104" s="49"/>
+      <c r="J104" s="50"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A105" s="51"/>
+      <c r="B105" s="131"/>
+      <c r="C105" s="73"/>
+      <c r="D105" s="73"/>
+      <c r="E105" s="73"/>
+      <c r="F105" s="73"/>
+      <c r="G105" s="73"/>
+      <c r="H105" s="73"/>
+      <c r="I105" s="49"/>
+      <c r="J105" s="50"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A106" s="51"/>
+      <c r="B106" s="132"/>
+      <c r="C106" s="45"/>
+      <c r="D106" s="45"/>
+      <c r="E106" s="45"/>
+      <c r="F106" s="45"/>
+      <c r="G106" s="45"/>
+      <c r="H106" s="81"/>
+      <c r="I106" s="65"/>
+      <c r="J106" s="50"/>
+    </row>
+    <row r="107" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A107" s="51"/>
+      <c r="B107" s="133"/>
+      <c r="C107" s="5"/>
+      <c r="D107" s="5"/>
+      <c r="E107" s="5"/>
+      <c r="F107" s="5"/>
+      <c r="G107" s="5"/>
+      <c r="H107" s="5"/>
+      <c r="I107" s="6"/>
+      <c r="J107" s="50"/>
+    </row>
+    <row r="108" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A108" s="51"/>
+      <c r="B108" s="134" t="s">
         <v>171</v>
       </c>
-      <c r="B104" s="6"/>
-      <c r="C104" s="6"/>
-      <c r="D104" s="6"/>
-      <c r="E104" s="6"/>
-      <c r="F104" s="6"/>
-      <c r="G104" s="6"/>
-      <c r="H104" s="7"/>
-    </row>
-    <row r="105" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A105" s="77" t="s">
+      <c r="C108" s="5"/>
+      <c r="D108" s="5"/>
+      <c r="E108" s="5"/>
+      <c r="F108" s="5"/>
+      <c r="G108" s="5"/>
+      <c r="H108" s="5"/>
+      <c r="I108" s="6"/>
+      <c r="J108" s="50"/>
+    </row>
+    <row r="109" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A109" s="51"/>
+      <c r="B109" s="135" t="s">
         <v>47</v>
       </c>
-      <c r="B105" s="78"/>
-      <c r="C105" s="78"/>
-      <c r="D105" s="78"/>
-      <c r="E105" s="78"/>
-      <c r="F105" s="78"/>
-      <c r="G105" s="78"/>
-      <c r="H105" s="79"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A106" s="61"/>
-      <c r="B106" s="40"/>
-      <c r="C106" s="80" t="s">
+      <c r="C109" s="77"/>
+      <c r="D109" s="77"/>
+      <c r="E109" s="77"/>
+      <c r="F109" s="77"/>
+      <c r="G109" s="77"/>
+      <c r="H109" s="77"/>
+      <c r="I109" s="78"/>
+      <c r="J109" s="50"/>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A110" s="51"/>
+      <c r="B110" s="136"/>
+      <c r="C110" s="39"/>
+      <c r="D110" s="79" t="s">
         <v>87</v>
       </c>
-      <c r="D106" s="80" t="s">
+      <c r="E110" s="79" t="s">
         <v>164</v>
       </c>
-      <c r="E106" s="105" t="s">
+      <c r="F110" s="102" t="s">
         <v>165</v>
       </c>
-      <c r="G106" s="82"/>
-      <c r="H106" s="83" t="s">
+      <c r="H110" s="81"/>
+      <c r="I110" s="82" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A107" s="123" t="s">
+      <c r="J110" s="50"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A111" s="51"/>
+      <c r="B111" s="137" t="s">
         <v>49</v>
       </c>
-      <c r="B107" s="124"/>
-      <c r="C107" s="124"/>
-      <c r="D107" s="124"/>
-      <c r="E107" s="124"/>
-      <c r="F107" s="124"/>
-      <c r="G107" s="82"/>
-      <c r="H107" s="66"/>
-    </row>
-    <row r="108" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A108" s="84" t="s">
+      <c r="C111" s="122"/>
+      <c r="D111" s="122"/>
+      <c r="E111" s="122"/>
+      <c r="F111" s="122"/>
+      <c r="G111" s="122"/>
+      <c r="H111" s="81"/>
+      <c r="I111" s="65"/>
+      <c r="J111" s="50"/>
+    </row>
+    <row r="112" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A112" s="51"/>
+      <c r="B112" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="B108" s="85"/>
-      <c r="C108" s="85"/>
-      <c r="D108" s="85"/>
-      <c r="E108" s="53" t="s">
+      <c r="C112" s="84"/>
+      <c r="D112" s="84"/>
+      <c r="E112" s="84"/>
+      <c r="F112" s="52" t="s">
         <v>145</v>
       </c>
-      <c r="F108" s="54"/>
-      <c r="G108" s="54"/>
-      <c r="H108" s="56"/>
-    </row>
-    <row r="109" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A109" s="47" t="s">
+      <c r="G112" s="53"/>
+      <c r="H112" s="53"/>
+      <c r="I112" s="55"/>
+      <c r="J112" s="50"/>
+    </row>
+    <row r="113" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A113" s="51"/>
+      <c r="B113" s="128" t="s">
         <v>52</v>
       </c>
-      <c r="B109" s="48"/>
-      <c r="C109" s="48"/>
-      <c r="D109" s="48"/>
-      <c r="E109" s="51"/>
-      <c r="H109" s="52"/>
-    </row>
-    <row r="110" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A110" s="47" t="s">
+      <c r="C113" s="47"/>
+      <c r="D113" s="47"/>
+      <c r="E113" s="47"/>
+      <c r="F113" s="50"/>
+      <c r="I113" s="51"/>
+      <c r="J113" s="50"/>
+    </row>
+    <row r="114" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A114" s="51"/>
+      <c r="B114" s="128" t="s">
         <v>53</v>
       </c>
-      <c r="B110" s="48"/>
-      <c r="C110" s="48"/>
-      <c r="D110" s="48"/>
-      <c r="E110" s="51"/>
-      <c r="H110" s="52"/>
-    </row>
-    <row r="111" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A111" s="47" t="s">
+      <c r="C114" s="47"/>
+      <c r="D114" s="47"/>
+      <c r="E114" s="47"/>
+      <c r="F114" s="50"/>
+      <c r="I114" s="51"/>
+      <c r="J114" s="50"/>
+    </row>
+    <row r="115" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A115" s="51"/>
+      <c r="B115" s="128" t="s">
         <v>88</v>
       </c>
-      <c r="B111" s="48"/>
-      <c r="C111" s="48"/>
-      <c r="D111" s="48"/>
-      <c r="E111" s="51"/>
-      <c r="H111" s="52"/>
-    </row>
-    <row r="112" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A112" s="71" t="s">
+      <c r="C115" s="47"/>
+      <c r="D115" s="47"/>
+      <c r="E115" s="47"/>
+      <c r="F115" s="50"/>
+      <c r="I115" s="51"/>
+      <c r="J115" s="50"/>
+    </row>
+    <row r="116" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A116" s="51"/>
+      <c r="B116" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="B112" s="72"/>
-      <c r="C112" s="72"/>
-      <c r="D112" s="72"/>
-      <c r="E112" s="86"/>
-      <c r="F112" s="69"/>
-      <c r="G112" s="69"/>
-      <c r="H112" s="70"/>
-    </row>
+      <c r="C116" s="71"/>
+      <c r="D116" s="71"/>
+      <c r="E116" s="71"/>
+      <c r="F116" s="85"/>
+      <c r="G116" s="68"/>
+      <c r="H116" s="68"/>
+      <c r="I116" s="69"/>
+      <c r="J116" s="50"/>
+    </row>
+    <row r="117" spans="1:10" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="118" spans="1:10" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="121" spans="1:10" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="122" spans="1:10" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="123" spans="1:10" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="124" spans="1:10" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="125" spans="1:10" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="126" spans="1:10" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="128" spans="1:10" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="129" hidden="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A107:F107"/>
-    <mergeCell ref="A73:D73"/>
-    <mergeCell ref="E73:H73"/>
-    <mergeCell ref="A43:F43"/>
-    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B111:G111"/>
+    <mergeCell ref="B77:E77"/>
+    <mergeCell ref="F77:I77"/>
+    <mergeCell ref="B43:G43"/>
+    <mergeCell ref="F14:I14"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.15748031496062992" bottom="0.15748031496062992" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="76" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
group by product (storage template) added
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement_Vessels.xlsx
+++ b/templates/Export_Agreement_Vessels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B889CF1-144A-4077-BB63-9CC4879C3552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCA4325-0B7C-46C5-94EC-DD0DA8B2AB28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-52882" yWindow="3045" windowWidth="13425" windowHeight="7800" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
@@ -974,7 +974,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1312,12 +1312,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1326,40 +1326,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2405,7 +2371,7 @@
   <dimension ref="A2:AB129"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A42" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3083,14 +3049,14 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" s="51"/>
-      <c r="B43" s="121" t="s">
+      <c r="B43" s="122" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="122"/>
-      <c r="D43" s="122"/>
-      <c r="E43" s="122"/>
-      <c r="F43" s="122"/>
-      <c r="G43" s="122"/>
+      <c r="C43" s="121"/>
+      <c r="D43" s="121"/>
+      <c r="E43" s="121"/>
+      <c r="F43" s="121"/>
+      <c r="G43" s="121"/>
       <c r="H43" s="81"/>
       <c r="I43" s="65"/>
       <c r="J43" s="50"/>
@@ -3307,7 +3273,7 @@
     </row>
     <row r="72" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72" s="51"/>
-      <c r="B72" s="126" t="s">
+      <c r="B72" s="88" t="s">
         <v>57</v>
       </c>
       <c r="C72" s="88"/>
@@ -3327,7 +3293,7 @@
     </row>
     <row r="73" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="51"/>
-      <c r="B73" s="127" t="s">
+      <c r="B73" s="44" t="s">
         <v>59</v>
       </c>
       <c r="C73" s="44"/>
@@ -3377,7 +3343,7 @@
     </row>
     <row r="76" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="51"/>
-      <c r="B76" s="128" t="s">
+      <c r="B76" s="47" t="s">
         <v>13</v>
       </c>
       <c r="C76" s="47"/>
@@ -3409,7 +3375,7 @@
     </row>
     <row r="78" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="51"/>
-      <c r="B78" s="129" t="s">
+      <c r="B78" s="94" t="s">
         <v>64</v>
       </c>
       <c r="C78" s="63" t="s">
@@ -3426,7 +3392,7 @@
     </row>
     <row r="79" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79" s="51"/>
-      <c r="B79" s="127" t="s">
+      <c r="B79" s="44" t="s">
         <v>66</v>
       </c>
       <c r="C79" s="93" t="s">
@@ -3443,7 +3409,7 @@
     </row>
     <row r="80" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80" s="51"/>
-      <c r="B80" s="129" t="s">
+      <c r="B80" s="94" t="s">
         <v>69</v>
       </c>
       <c r="C80" s="94" t="s">
@@ -3477,7 +3443,7 @@
     </row>
     <row r="82" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="51"/>
-      <c r="B82" s="130" t="s">
+      <c r="B82" t="s">
         <v>154</v>
       </c>
       <c r="D82" s="95"/>
@@ -3492,7 +3458,6 @@
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A83" s="51"/>
-      <c r="B83" s="130"/>
       <c r="D83" s="68"/>
       <c r="E83" s="96"/>
       <c r="F83" s="70" t="s">
@@ -3531,7 +3496,7 @@
     </row>
     <row r="85" spans="1:18" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85" s="51"/>
-      <c r="B85" s="131" t="s">
+      <c r="B85" s="73" t="s">
         <v>35</v>
       </c>
       <c r="C85" s="73" t="s">
@@ -3559,7 +3524,7 @@
     </row>
     <row r="86" spans="1:18" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A86" s="51"/>
-      <c r="B86" s="131"/>
+      <c r="B86" s="73"/>
       <c r="C86" s="73"/>
       <c r="D86" s="73"/>
       <c r="E86" s="73"/>
@@ -3571,7 +3536,7 @@
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A87" s="51"/>
-      <c r="B87" s="131"/>
+      <c r="B87" s="73"/>
       <c r="C87" s="73"/>
       <c r="D87" s="73"/>
       <c r="E87" s="73"/>
@@ -3583,7 +3548,7 @@
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A88" s="51"/>
-      <c r="B88" s="131"/>
+      <c r="B88" s="73"/>
       <c r="C88" s="73"/>
       <c r="D88" s="73"/>
       <c r="E88" s="73"/>
@@ -3602,7 +3567,7 @@
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A90" s="51"/>
-      <c r="B90" s="131"/>
+      <c r="B90" s="73"/>
       <c r="C90" s="73"/>
       <c r="D90" s="73"/>
       <c r="E90" s="73"/>
@@ -3615,7 +3580,7 @@
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A91" s="51"/>
-      <c r="B91" s="131"/>
+      <c r="B91" s="73"/>
       <c r="C91" s="73"/>
       <c r="D91" s="73"/>
       <c r="E91" s="73"/>
@@ -3627,7 +3592,7 @@
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A92" s="51"/>
-      <c r="B92" s="131"/>
+      <c r="B92" s="73"/>
       <c r="C92" s="73"/>
       <c r="D92" s="73"/>
       <c r="E92" s="73"/>
@@ -3639,7 +3604,7 @@
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A93" s="51"/>
-      <c r="B93" s="131"/>
+      <c r="B93" s="73"/>
       <c r="C93" s="73"/>
       <c r="D93" s="73"/>
       <c r="E93" s="73"/>
@@ -3651,7 +3616,7 @@
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A94" s="51"/>
-      <c r="B94" s="131"/>
+      <c r="B94" s="73"/>
       <c r="C94" s="73"/>
       <c r="D94" s="73"/>
       <c r="E94" s="73"/>
@@ -3663,7 +3628,7 @@
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A95" s="51"/>
-      <c r="B95" s="131"/>
+      <c r="B95" s="73"/>
       <c r="C95" s="73"/>
       <c r="D95" s="73"/>
       <c r="E95" s="73"/>
@@ -3675,7 +3640,7 @@
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A96" s="51"/>
-      <c r="B96" s="131"/>
+      <c r="B96" s="73"/>
       <c r="C96" s="73"/>
       <c r="D96" s="73"/>
       <c r="E96" s="73"/>
@@ -3687,7 +3652,7 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A97" s="51"/>
-      <c r="B97" s="131"/>
+      <c r="B97" s="73"/>
       <c r="C97" s="73"/>
       <c r="D97" s="73"/>
       <c r="E97" s="73"/>
@@ -3699,7 +3664,7 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A98" s="51"/>
-      <c r="B98" s="131"/>
+      <c r="B98" s="73"/>
       <c r="C98" s="73"/>
       <c r="D98" s="73"/>
       <c r="E98" s="73"/>
@@ -3711,7 +3676,7 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A99" s="51"/>
-      <c r="B99" s="131"/>
+      <c r="B99" s="73"/>
       <c r="C99" s="73"/>
       <c r="D99" s="73"/>
       <c r="E99" s="73"/>
@@ -3723,7 +3688,7 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A100" s="51"/>
-      <c r="B100" s="131"/>
+      <c r="B100" s="73"/>
       <c r="C100" s="73"/>
       <c r="D100" s="73"/>
       <c r="E100" s="73"/>
@@ -3735,7 +3700,7 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A101" s="51"/>
-      <c r="B101" s="131"/>
+      <c r="B101" s="73"/>
       <c r="C101" s="73"/>
       <c r="D101" s="73"/>
       <c r="E101" s="73"/>
@@ -3746,7 +3711,7 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A102" s="51"/>
-      <c r="B102" s="131"/>
+      <c r="B102" s="73"/>
       <c r="C102" s="73"/>
       <c r="D102" s="73"/>
       <c r="E102" s="73"/>
@@ -3758,7 +3723,7 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A103" s="51"/>
-      <c r="B103" s="131"/>
+      <c r="B103" s="73"/>
       <c r="C103" s="73"/>
       <c r="D103" s="73"/>
       <c r="E103" s="73"/>
@@ -3770,7 +3735,7 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A104" s="51"/>
-      <c r="B104" s="131"/>
+      <c r="B104" s="73"/>
       <c r="C104" s="73"/>
       <c r="D104" s="73"/>
       <c r="E104" s="73"/>
@@ -3782,7 +3747,7 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A105" s="51"/>
-      <c r="B105" s="131"/>
+      <c r="B105" s="73"/>
       <c r="C105" s="73"/>
       <c r="D105" s="73"/>
       <c r="E105" s="73"/>
@@ -3794,7 +3759,7 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A106" s="51"/>
-      <c r="B106" s="132"/>
+      <c r="B106" s="45"/>
       <c r="C106" s="45"/>
       <c r="D106" s="45"/>
       <c r="E106" s="45"/>
@@ -3806,7 +3771,7 @@
     </row>
     <row r="107" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A107" s="51"/>
-      <c r="B107" s="133"/>
+      <c r="B107" s="5"/>
       <c r="C107" s="5"/>
       <c r="D107" s="5"/>
       <c r="E107" s="5"/>
@@ -3818,7 +3783,7 @@
     </row>
     <row r="108" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A108" s="51"/>
-      <c r="B108" s="134" t="s">
+      <c r="B108" s="3" t="s">
         <v>171</v>
       </c>
       <c r="C108" s="5"/>
@@ -3832,7 +3797,7 @@
     </row>
     <row r="109" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A109" s="51"/>
-      <c r="B109" s="135" t="s">
+      <c r="B109" s="77" t="s">
         <v>47</v>
       </c>
       <c r="C109" s="77"/>
@@ -3846,7 +3811,7 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A110" s="51"/>
-      <c r="B110" s="136"/>
+      <c r="B110" s="39"/>
       <c r="C110" s="39"/>
       <c r="D110" s="79" t="s">
         <v>87</v>
@@ -3865,14 +3830,14 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A111" s="51"/>
-      <c r="B111" s="137" t="s">
+      <c r="B111" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="C111" s="122"/>
-      <c r="D111" s="122"/>
-      <c r="E111" s="122"/>
-      <c r="F111" s="122"/>
-      <c r="G111" s="122"/>
+      <c r="C111" s="121"/>
+      <c r="D111" s="121"/>
+      <c r="E111" s="121"/>
+      <c r="F111" s="121"/>
+      <c r="G111" s="121"/>
       <c r="H111" s="81"/>
       <c r="I111" s="65"/>
       <c r="J111" s="50"/>
@@ -3895,7 +3860,7 @@
     </row>
     <row r="113" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A113" s="51"/>
-      <c r="B113" s="128" t="s">
+      <c r="B113" s="47" t="s">
         <v>52</v>
       </c>
       <c r="C113" s="47"/>
@@ -3907,7 +3872,7 @@
     </row>
     <row r="114" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A114" s="51"/>
-      <c r="B114" s="128" t="s">
+      <c r="B114" s="47" t="s">
         <v>53</v>
       </c>
       <c r="C114" s="47"/>
@@ -3919,7 +3884,7 @@
     </row>
     <row r="115" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A115" s="51"/>
-      <c r="B115" s="128" t="s">
+      <c r="B115" s="47" t="s">
         <v>88</v>
       </c>
       <c r="C115" s="47"/>

</xml_diff>

<commit_message>
working on export agreement fca template implementation, fixing merge cells bug
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement_Vessels.xlsx
+++ b/templates/Export_Agreement_Vessels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B59F82A-0076-46E9-AD71-C624368D293B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CEFC8A-8C64-4CF6-8D90-4170814A8A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="15795" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="-57697" yWindow="-277" windowWidth="28995" windowHeight="15795" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
@@ -974,7 +974,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1317,15 +1317,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1647,8 +1638,8 @@
   </sheetPr>
   <dimension ref="A1:W85"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A12" zoomScale="140" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A29" zoomScale="140" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2370,14 +2361,14 @@
   </sheetPr>
   <dimension ref="A2:AB129"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A8" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A70" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.53125" customWidth="1"/>
-    <col min="2" max="2" width="14.06640625" customWidth="1"/>
+    <col min="2" max="2" width="15.265625" customWidth="1"/>
     <col min="3" max="3" width="20.1328125" customWidth="1"/>
     <col min="4" max="4" width="26.06640625" customWidth="1"/>
     <col min="5" max="5" width="11.06640625" customWidth="1"/>
@@ -2608,12 +2599,12 @@
       <c r="A14" s="51"/>
       <c r="B14" s="50"/>
       <c r="E14" s="65"/>
-      <c r="F14" s="123" t="s">
+      <c r="F14" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="124"/>
-      <c r="H14" s="124"/>
-      <c r="I14" s="125"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="59"/>
       <c r="J14" s="50"/>
     </row>
     <row r="15" spans="1:28" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
@@ -3922,7 +3913,7 @@
     <row r="128" spans="1:10" hidden="1" x14ac:dyDescent="0.45"/>
     <row r="129" hidden="1" x14ac:dyDescent="0.45"/>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="8">
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="F8:I8"/>
     <mergeCell ref="F5:G5"/>
@@ -3931,7 +3922,6 @@
     <mergeCell ref="B77:E77"/>
     <mergeCell ref="F77:I77"/>
     <mergeCell ref="B43:G43"/>
-    <mergeCell ref="F14:I14"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.15748031496062992" bottom="0.15748031496062992" header="0" footer="0"/>

</xml_diff>

<commit_message>
template port_letter fixed (names added for banner)
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement_Vessels.xlsx
+++ b/templates/Export_Agreement_Vessels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CEFC8A-8C64-4CF6-8D90-4170814A8A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E581A251-5A35-4CA4-A2A1-116471F365DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57697" yWindow="-277" windowWidth="28995" windowHeight="15795" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="15796" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
@@ -1630,6 +1630,24 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="700" row="2">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{03E4E8DC-2682-4AD3-AE41-6DCE65612C25}">
+  <we:reference id="5dbca137-d02b-4283-adec-e6f28aeb3ed7" version="1.0.0.0" store="developer" storeType="Registry"/>
+  <we:alternateReferences/>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B05EB69-7436-401E-967C-BE559ABF33B1}">
   <sheetPr>
@@ -1638,8 +1656,8 @@
   </sheetPr>
   <dimension ref="A1:W85"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A29" zoomScale="140" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A12" zoomScale="140" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2361,7 +2379,7 @@
   </sheetPr>
   <dimension ref="A2:AB129"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A70" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A70" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
       <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
checkout for previous version
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement_Vessels.xlsx
+++ b/templates/Export_Agreement_Vessels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E581A251-5A35-4CA4-A2A1-116471F365DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72E14E8-5CC7-4834-9D91-3ED60D26875B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="15796" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
@@ -1656,8 +1656,8 @@
   </sheetPr>
   <dimension ref="A1:W85"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A12" zoomScale="140" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A12" zoomScale="140" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2379,8 +2379,8 @@
   </sheetPr>
   <dimension ref="A2:AB129"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A70" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A70" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
EXW declaration condition added to tmp, + some minor tmp fixes
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement_Vessels.xlsx
+++ b/templates/Export_Agreement_Vessels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72E14E8-5CC7-4834-9D91-3ED60D26875B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B023E1BE-1330-4376-A617-3DB6C2072643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="7890" yWindow="3713" windowWidth="14385" windowHeight="7484" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
@@ -659,9 +659,6 @@
     <t>34 247,50 USD</t>
   </si>
   <si>
-    <t>432 шт/</t>
-  </si>
-  <si>
     <t xml:space="preserve">9,735 тн </t>
   </si>
   <si>
@@ -692,6 +689,9 @@
   </si>
   <si>
     <t>СТРАНА ПРОИСХОЖДЕНИЯ РОССИЯ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">432 шт/ </t>
   </si>
 </sst>
 </file>
@@ -1255,9 +1255,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
@@ -1280,6 +1277,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1656,7 +1656,7 @@
   </sheetPr>
   <dimension ref="A1:W85"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A12" zoomScale="140" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A7" zoomScale="140" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -1752,11 +1752,11 @@
       <c r="U3" s="8"/>
       <c r="V3" s="8"/>
     </row>
-    <row r="4" spans="1:22" s="106" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="107" t="s">
+    <row r="4" spans="1:22" s="105" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="106" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="108" t="s">
+      <c r="B4" s="107" t="s">
         <v>92</v>
       </c>
       <c r="F4" s="10"/>
@@ -1946,7 +1946,7 @@
     </row>
     <row r="17" spans="1:22" ht="35.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>158</v>
@@ -2123,11 +2123,11 @@
       <c r="V26" s="34"/>
     </row>
     <row r="27" spans="1:22" ht="124.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="110" t="s">
+      <c r="A27" s="109" t="s">
+        <v>168</v>
+      </c>
+      <c r="B27" s="109" t="s">
         <v>169</v>
-      </c>
-      <c r="B27" s="110" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.45">
@@ -2299,48 +2299,48 @@
       </c>
     </row>
     <row r="49" spans="1:2" ht="10.9" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="109"/>
-      <c r="B49" s="109"/>
+      <c r="A49" s="108"/>
+      <c r="B49" s="108"/>
     </row>
     <row r="50" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="109"/>
-      <c r="B50" s="109"/>
+      <c r="A50" s="108"/>
+      <c r="B50" s="108"/>
     </row>
     <row r="51" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="109"/>
-      <c r="B51" s="109"/>
+      <c r="A51" s="108"/>
+      <c r="B51" s="108"/>
     </row>
     <row r="52" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="109"/>
-      <c r="B52" s="109"/>
+      <c r="A52" s="108"/>
+      <c r="B52" s="108"/>
     </row>
     <row r="53" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="109"/>
-      <c r="B53" s="109"/>
+      <c r="A53" s="108"/>
+      <c r="B53" s="108"/>
     </row>
     <row r="54" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="109"/>
-      <c r="B54" s="109"/>
+      <c r="A54" s="108"/>
+      <c r="B54" s="108"/>
     </row>
     <row r="55" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="109"/>
-      <c r="B55" s="109"/>
+      <c r="A55" s="108"/>
+      <c r="B55" s="108"/>
     </row>
     <row r="56" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="109"/>
-      <c r="B56" s="109"/>
+      <c r="A56" s="108"/>
+      <c r="B56" s="108"/>
     </row>
     <row r="57" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="109"/>
-      <c r="B57" s="109"/>
+      <c r="A57" s="108"/>
+      <c r="B57" s="108"/>
     </row>
     <row r="58" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="109"/>
-      <c r="B58" s="109"/>
+      <c r="A58" s="108"/>
+      <c r="B58" s="108"/>
     </row>
     <row r="59" spans="1:2" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="109"/>
-      <c r="B59" s="109"/>
+      <c r="A59" s="108"/>
+      <c r="B59" s="108"/>
     </row>
     <row r="60" spans="1:2" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="61" spans="1:2" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2379,8 +2379,8 @@
   </sheetPr>
   <dimension ref="A2:AB129"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A70" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A92" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2389,7 +2389,7 @@
     <col min="2" max="2" width="15.265625" customWidth="1"/>
     <col min="3" max="3" width="20.1328125" customWidth="1"/>
     <col min="4" max="4" width="26.06640625" customWidth="1"/>
-    <col min="5" max="5" width="11.06640625" customWidth="1"/>
+    <col min="5" max="5" width="12.796875" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" customWidth="1"/>
@@ -2405,7 +2405,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:28" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="102" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="37"/>
@@ -2462,7 +2462,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:28" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="51"/>
       <c r="B5" s="42" t="s">
         <v>152</v>
@@ -2517,7 +2517,7 @@
     <row r="8" spans="1:28" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="51"/>
       <c r="B8" s="111" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C8" s="112"/>
       <c r="D8" s="112"/>
@@ -2639,10 +2639,10 @@
       <c r="E15" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="105" t="s">
+      <c r="F15" s="104" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="105"/>
+      <c r="G15" s="104"/>
       <c r="H15" s="98" t="s">
         <v>33</v>
       </c>
@@ -3269,7 +3269,7 @@
       <c r="E70" s="44"/>
     </row>
     <row r="71" spans="1:10" ht="28.15" customHeight="1" x14ac:dyDescent="0.85">
-      <c r="B71" s="104" t="s">
+      <c r="B71" s="103" t="s">
         <v>56</v>
       </c>
       <c r="C71" s="86"/>
@@ -3793,7 +3793,7 @@
     <row r="108" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A108" s="51"/>
       <c r="B108" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C108" s="5"/>
       <c r="D108" s="5"/>
@@ -3826,14 +3826,14 @@
         <v>87</v>
       </c>
       <c r="E110" s="79" t="s">
+        <v>171</v>
+      </c>
+      <c r="F110" s="110" t="s">
         <v>164</v>
-      </c>
-      <c r="F110" s="102" t="s">
-        <v>165</v>
       </c>
       <c r="H110" s="81"/>
       <c r="I110" s="82" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J110" s="50"/>
     </row>
@@ -3943,6 +3943,6 @@
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.15748031496062992" bottom="0.15748031496062992" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="72" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>